<commit_message>
did binary and hierarchical testing
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_final.xlsx
+++ b/models/evaluations/evaluation_prompts_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8E657E-A490-714B-8781-5D3DBE2EE331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15B4803-8677-8C40-8549-B75D63EC0E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22360" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="127">
   <si>
     <t>prompt description</t>
   </si>
@@ -405,9 +405,6 @@
     <t>summary enriched_kw_0.2test_gpt-3.5</t>
   </si>
   <si>
-    <t>summary enriched_0.2test_gpt-3.5</t>
-  </si>
-  <si>
     <t>Binary</t>
   </si>
   <si>
@@ -472,6 +469,27 @@
   </si>
   <si>
     <t>keywords vs w/o keywords: which performs better</t>
+  </si>
+  <si>
+    <t>summary enriched_0.2test_gpt-3.5 (w/o new Fuzzy Match)</t>
+  </si>
+  <si>
+    <t>summary enriched_kw_0.2test_gpt-3.5 (with fuzzy Match)</t>
+  </si>
+  <si>
+    <t>ICL (few-shot), random samples</t>
+  </si>
+  <si>
+    <t>ICL (few-shot): closest neighbours from the train dataset to each test example</t>
+  </si>
+  <si>
+    <t>Hierarchical</t>
+  </si>
+  <si>
+    <t>P1_Hierarchical</t>
+  </si>
+  <si>
+    <t>P2_Hierarchical</t>
   </si>
 </sst>
 </file>
@@ -664,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -705,6 +723,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,7 +1069,7 @@
   <dimension ref="A1:AU62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="87" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,16 +1095,16 @@
   <sheetData>
     <row r="1" spans="2:47" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" t="s">
         <v>112</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
+        <v>114</v>
+      </c>
+      <c r="X1" t="s">
         <v>113</v>
-      </c>
-      <c r="R1" t="s">
-        <v>115</v>
-      </c>
-      <c r="X1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
@@ -1093,19 +1114,19 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="Q2" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
       <c r="T2" s="17"/>
       <c r="U2" s="6"/>
       <c r="W2" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X2" s="21"/>
       <c r="Y2" s="21"/>
@@ -1409,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
         <v>96</v>
@@ -2191,7 +2212,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22">
         <v>0.57200399999999996</v>
@@ -2241,7 +2262,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
         <v>96</v>
@@ -2294,7 +2315,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
         <v>96</v>
@@ -2420,7 +2441,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
         <v>96</v>
@@ -2493,7 +2514,7 @@
         <v>90</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
         <v>96</v>
@@ -2594,10 +2615,10 @@
     <row r="29" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A29" s="26"/>
       <c r="B29" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29">
         <v>0.57575100000000001</v>
@@ -2609,7 +2630,7 @@
         <v>0.421572</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K29">
         <v>0.59193499999999999</v>
@@ -2621,7 +2642,7 @@
         <v>0.42186299999999999</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q29">
         <v>0.52521300000000004</v>
@@ -2633,17 +2654,17 @@
         <v>0.32766000000000001</v>
       </c>
       <c r="U29" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AG29" s="2"/>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
       <c r="B30" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30">
         <v>0.604819</v>
@@ -2655,7 +2676,7 @@
         <v>0.44495600000000002</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K30">
         <v>0.60010799999999997</v>
@@ -2667,7 +2688,7 @@
         <v>0.43686399999999997</v>
       </c>
       <c r="O30" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q30">
         <v>0.55145900000000003</v>
@@ -2679,7 +2700,7 @@
         <v>0.39478099999999999</v>
       </c>
       <c r="U30" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V30" s="16"/>
       <c r="W30">
@@ -2698,10 +2719,10 @@
     <row r="34" spans="2:25" x14ac:dyDescent="0.2">
       <c r="K34" s="1"/>
       <c r="Q34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="W34" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X34" s="27"/>
       <c r="Y34" s="27"/>
@@ -2723,15 +2744,15 @@
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2842,6 +2863,15 @@
         <v>6</v>
       </c>
       <c r="C39" s="11"/>
+      <c r="E39">
+        <v>0.91222199999999998</v>
+      </c>
+      <c r="F39">
+        <v>0.91573000000000004</v>
+      </c>
+      <c r="G39">
+        <v>0.90570700000000004</v>
+      </c>
       <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
       <c r="S39" s="12"/>
@@ -2853,10 +2883,19 @@
       <c r="Y39" s="12"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B40" s="9" t="s">
-        <v>20</v>
+      <c r="B40" s="30" t="s">
+        <v>7</v>
       </c>
       <c r="C40" s="11"/>
+      <c r="E40">
+        <v>0.94818100000000005</v>
+      </c>
+      <c r="F40">
+        <v>0.94569300000000001</v>
+      </c>
+      <c r="G40">
+        <v>0.94666399999999995</v>
+      </c>
       <c r="Q40">
         <v>0.55821900000000002</v>
       </c>
@@ -2880,10 +2919,8 @@
       </c>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B41" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="11"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
       <c r="Q41">
         <v>0.53802099999999997</v>
       </c>
@@ -2907,10 +2944,8 @@
       </c>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B42" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="11"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
       <c r="Q42">
         <v>0.53802099999999997</v>
       </c>
@@ -2934,10 +2969,8 @@
       </c>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B43" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="11"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
       <c r="Q43">
         <v>0.58662300000000001</v>
       </c>
@@ -2961,10 +2994,8 @@
       </c>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B44" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="11"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
       <c r="Q44" s="12"/>
       <c r="R44" s="12"/>
       <c r="S44" s="12"/>
@@ -2976,10 +3007,8 @@
       <c r="Y44" s="12"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B45" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="11"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
       <c r="Q45">
         <v>0.56189900000000004</v>
       </c>
@@ -3003,10 +3032,19 @@
       </c>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B46" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="11"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46">
+        <v>0.27852900000000003</v>
+      </c>
+      <c r="F46">
+        <v>0.19802</v>
+      </c>
+      <c r="G46">
+        <v>0.15489900000000001</v>
+      </c>
       <c r="Q46">
         <v>0.54681400000000002</v>
       </c>
@@ -3030,10 +3068,19 @@
       </c>
     </row>
     <row r="47" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B47" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="11"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47">
+        <v>0.31304599999999999</v>
+      </c>
+      <c r="F47">
+        <v>0.32425700000000002</v>
+      </c>
+      <c r="G47">
+        <v>0.31349399999999999</v>
+      </c>
       <c r="Q47">
         <v>0.62534100000000004</v>
       </c>
@@ -3057,10 +3104,8 @@
       </c>
     </row>
     <row r="48" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B48" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="11"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
       <c r="Q48">
         <v>0.57320499999999996</v>
       </c>
@@ -3084,10 +3129,9 @@
       </c>
     </row>
     <row r="49" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B49" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="11"/>
+      <c r="B49" s="18" t="s">
+        <v>124</v>
+      </c>
       <c r="Q49">
         <v>0.44090699999999999</v>
       </c>
@@ -3111,10 +3155,21 @@
       </c>
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="11"/>
+      <c r="B50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K50" t="s">
+        <v>126</v>
+      </c>
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
       <c r="S50" s="12"/>
@@ -3127,9 +3182,30 @@
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B51" s="8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C51" s="11"/>
+      <c r="E51">
+        <v>0.43861299999999998</v>
+      </c>
+      <c r="F51">
+        <v>0.310861</v>
+      </c>
+      <c r="G51">
+        <v>0.25757999999999998</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K51">
+        <v>0.58002900000000002</v>
+      </c>
+      <c r="L51">
+        <v>0.50749100000000003</v>
+      </c>
+      <c r="M51">
+        <v>0.50221300000000002</v>
+      </c>
       <c r="Q51">
         <v>0.52873999999999999</v>
       </c>
@@ -3153,10 +3229,31 @@
       </c>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B52" s="9" t="s">
-        <v>17</v>
+      <c r="B52" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="C52" s="11"/>
+      <c r="E52">
+        <v>0.44281799999999999</v>
+      </c>
+      <c r="F52">
+        <v>0.31273400000000001</v>
+      </c>
+      <c r="G52">
+        <v>0.26475300000000002</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K52">
+        <v>0.58660100000000004</v>
+      </c>
+      <c r="L52">
+        <v>0.503745</v>
+      </c>
+      <c r="M52">
+        <v>0.499114</v>
+      </c>
       <c r="Q52">
         <v>0.547925</v>
       </c>
@@ -3180,10 +3277,31 @@
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B53" s="8" t="s">
-        <v>18</v>
+      <c r="B53" s="30" t="s">
+        <v>7</v>
       </c>
       <c r="C53" s="11"/>
+      <c r="E53">
+        <v>0.50392899999999996</v>
+      </c>
+      <c r="F53">
+        <v>0.34644200000000003</v>
+      </c>
+      <c r="G53">
+        <v>0.29471199999999997</v>
+      </c>
+      <c r="I53" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53">
+        <v>0.61691499999999999</v>
+      </c>
+      <c r="L53">
+        <v>0.550562</v>
+      </c>
+      <c r="M53">
+        <v>0.54048099999999999</v>
+      </c>
       <c r="Q53">
         <v>0.46595500000000001</v>
       </c>
@@ -3207,10 +3325,8 @@
       </c>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B54" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="11"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
       <c r="Q54">
         <v>0.541269</v>
       </c>
@@ -3234,10 +3350,8 @@
       </c>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B55" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="11"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
       <c r="Q55">
         <v>0.57905399999999996</v>
       </c>
@@ -3261,10 +3375,8 @@
       </c>
     </row>
     <row r="56" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B56" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="11"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
       <c r="Q56">
         <v>0.58247599999999999</v>
       </c>
@@ -3288,10 +3400,8 @@
       </c>
     </row>
     <row r="57" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="11"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
       <c r="Q57">
         <v>0.61878200000000005</v>
       </c>
@@ -3315,10 +3425,8 @@
       </c>
     </row>
     <row r="58" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" s="11"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
       <c r="Q58">
         <v>0.58768200000000004</v>
       </c>
@@ -3342,10 +3450,8 @@
       </c>
     </row>
     <row r="59" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B59" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59" s="11"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
       <c r="Q59">
         <v>0.54432199999999997</v>
       </c>
@@ -3369,10 +3475,8 @@
       </c>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B60" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="11"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
       <c r="Q60">
         <v>0.51415699999999998</v>
       </c>
@@ -3396,21 +3500,17 @@
       </c>
     </row>
     <row r="61" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B61" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="11"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
       <c r="U61" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="U62" s="25" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B62" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="11"/>
-      <c r="U62" s="25" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -5368,13 +5468,13 @@
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed ICL to enriched with kw
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_final.xlsx
+++ b/models/evaluations/evaluation_prompts_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D01375-08AA-0E49-A343-5CD09C27A60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBA60E3-165B-E84A-82A4-251E60342B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22360" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +630,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -682,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -708,6 +714,12 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,17 +727,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1066,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
-  <dimension ref="A1:AU62"/>
+  <dimension ref="B1:AU62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="87" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="87" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1118,35 +1120,35 @@
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
       <c r="T2" s="17"/>
       <c r="U2" s="6"/>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
       <c r="Z2" s="17"/>
-      <c r="AC2" s="21" t="s">
+      <c r="AC2" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-      <c r="AS2" s="21"/>
-      <c r="AT2" s="21"/>
-      <c r="AU2" s="21"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AS2" s="25"/>
+      <c r="AT2" s="25"/>
+      <c r="AU2" s="25"/>
     </row>
     <row r="3" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
@@ -1364,21 +1366,21 @@
       <c r="D6" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
       <c r="O6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
       <c r="T6" s="2"/>
       <c r="U6" s="9" t="s">
         <v>20</v>
@@ -1400,21 +1402,21 @@
       <c r="D7" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
       <c r="O7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
       <c r="U7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1653,21 +1655,21 @@
       <c r="D12" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
       <c r="I12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
       <c r="O12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
       <c r="U12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1889,7 @@
       <c r="F16">
         <v>0.54119899999999999</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="23">
         <v>0.53234800000000004</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -1925,19 +1927,19 @@
       <c r="X16">
         <v>0.60299599999999998</v>
       </c>
-      <c r="Y16" s="29">
+      <c r="Y16" s="23">
         <v>0.59994999999999998</v>
       </c>
       <c r="AA16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AC16" s="26">
+      <c r="AC16">
         <v>0.70457400000000003</v>
       </c>
-      <c r="AD16" s="26">
+      <c r="AD16">
         <v>0.53712899999999997</v>
       </c>
-      <c r="AE16" s="26">
+      <c r="AE16">
         <v>0.57348399999999999</v>
       </c>
       <c r="AG16" s="2"/>
@@ -1947,7 +1949,7 @@
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2018,7 @@
       <c r="AM17" s="8"/>
       <c r="AR17" s="8"/>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
@@ -2026,21 +2028,21 @@
       <c r="D18" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
       <c r="I18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
       <c r="O18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
       <c r="U18" s="9" t="s">
         <v>17</v>
       </c>
@@ -2051,7 +2053,7 @@
       <c r="AM18" s="9"/>
       <c r="AR18" s="9"/>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
@@ -2104,7 +2106,7 @@
       <c r="AM19" s="8"/>
       <c r="AR19" s="8"/>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>92</v>
       </c>
@@ -2157,7 +2159,7 @@
       <c r="AM20" s="8"/>
       <c r="AR20" s="8"/>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -2207,7 +2209,7 @@
       <c r="AM21" s="8"/>
       <c r="AR21" s="8"/>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
@@ -2257,7 +2259,7 @@
       <c r="AM22" s="8"/>
       <c r="AR22" s="8"/>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
@@ -2310,7 +2312,7 @@
       <c r="AM23" s="8"/>
       <c r="AR23" s="8"/>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2365,7 @@
       <c r="AM24" s="8"/>
       <c r="AR24" s="8"/>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2373,7 +2375,7 @@
       <c r="D25" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="23">
         <v>0.63638499999999998</v>
       </c>
       <c r="F25">
@@ -2436,7 +2438,7 @@
       <c r="AM25" s="8"/>
       <c r="AR25" s="8"/>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -2452,7 +2454,7 @@
       <c r="F26">
         <v>0.52808999999999995</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="23">
         <v>0.518258</v>
       </c>
       <c r="I26" s="8" t="s">
@@ -2490,7 +2492,7 @@
       <c r="X26">
         <v>0.60112399999999999</v>
       </c>
-      <c r="Y26" s="29">
+      <c r="Y26" s="23">
         <v>0.59575299999999998</v>
       </c>
       <c r="AA26" s="8" t="s">
@@ -2509,7 +2511,7 @@
       <c r="AM26" s="8"/>
       <c r="AR26" s="8"/>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>90</v>
       </c>
@@ -2562,7 +2564,7 @@
       <c r="AM27" s="8"/>
       <c r="AR27" s="8"/>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>91</v>
       </c>
@@ -2612,8 +2614,7 @@
       <c r="AM28" s="8"/>
       <c r="AR28" s="8"/>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
+    <row r="29" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B29" s="8" t="s">
         <v>106</v>
       </c>
@@ -2658,9 +2659,8 @@
       </c>
       <c r="AG29" s="2"/>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A30" s="26"/>
-      <c r="B30" s="25" t="s">
+    <row r="30" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B30" s="22" t="s">
         <v>107</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -2675,7 +2675,7 @@
       <c r="G30" s="14">
         <v>0.44495600000000002</v>
       </c>
-      <c r="I30" s="25" t="s">
+      <c r="I30" s="22" t="s">
         <v>107</v>
       </c>
       <c r="K30">
@@ -2687,7 +2687,7 @@
       <c r="M30">
         <v>0.43686399999999997</v>
       </c>
-      <c r="O30" s="25" t="s">
+      <c r="O30" s="22" t="s">
         <v>107</v>
       </c>
       <c r="Q30">
@@ -2699,7 +2699,7 @@
       <c r="S30">
         <v>0.39478099999999999</v>
       </c>
-      <c r="U30" s="25" t="s">
+      <c r="U30" s="22" t="s">
         <v>107</v>
       </c>
       <c r="V30" s="16"/>
@@ -2721,11 +2721,11 @@
       <c r="Q34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="W34" s="27" t="s">
+      <c r="W34" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="X34" s="27"/>
-      <c r="Y34" s="27"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="24"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.2">
       <c r="K35" s="1"/>
@@ -2883,7 +2883,7 @@
       <c r="Y39" s="12"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="11"/>
@@ -2919,8 +2919,7 @@
       </c>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B41" s="31"/>
-      <c r="C41" s="32"/>
+      <c r="B41" s="5"/>
       <c r="Q41">
         <v>0.53802099999999997</v>
       </c>
@@ -2944,8 +2943,6 @@
       </c>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
       <c r="Q42">
         <v>0.53802099999999997</v>
       </c>
@@ -2969,8 +2966,6 @@
       </c>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
       <c r="Q43">
         <v>0.58662300000000001</v>
       </c>
@@ -2994,8 +2989,6 @@
       </c>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
       <c r="Q44" s="12"/>
       <c r="R44" s="12"/>
       <c r="S44" s="12"/>
@@ -3007,8 +3000,6 @@
       <c r="Y44" s="12"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
       <c r="Q45">
         <v>0.56189900000000004</v>
       </c>
@@ -3032,8 +3023,8 @@
       </c>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B46" s="31"/>
-      <c r="C46" s="32" t="s">
+      <c r="B46" s="5"/>
+      <c r="C46" s="28" t="s">
         <v>123</v>
       </c>
       <c r="E46">
@@ -3068,8 +3059,7 @@
       </c>
     </row>
     <row r="47" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32" t="s">
+      <c r="C47" s="28" t="s">
         <v>122</v>
       </c>
       <c r="E47">
@@ -3104,8 +3094,6 @@
       </c>
     </row>
     <row r="48" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
       <c r="Q48">
         <v>0.57320499999999996</v>
       </c>
@@ -3277,7 +3265,7 @@
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="11"/>
@@ -3290,7 +3278,7 @@
       <c r="G53">
         <v>0.29471199999999997</v>
       </c>
-      <c r="I53" s="30" t="s">
+      <c r="I53" s="8" t="s">
         <v>7</v>
       </c>
       <c r="K53">
@@ -3299,7 +3287,7 @@
       <c r="L53">
         <v>0.550562</v>
       </c>
-      <c r="M53" s="29">
+      <c r="M53" s="23">
         <v>0.54048099999999999</v>
       </c>
       <c r="Q53">
@@ -3325,8 +3313,6 @@
       </c>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
       <c r="Q54">
         <v>0.541269</v>
       </c>
@@ -3350,8 +3336,6 @@
       </c>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
       <c r="Q55">
         <v>0.57905399999999996</v>
       </c>
@@ -3375,8 +3359,6 @@
       </c>
     </row>
     <row r="56" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
       <c r="Q56">
         <v>0.58247599999999999</v>
       </c>
@@ -3400,8 +3382,6 @@
       </c>
     </row>
     <row r="57" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="32"/>
-      <c r="C57" s="32"/>
       <c r="Q57">
         <v>0.61878200000000005</v>
       </c>
@@ -3425,8 +3405,6 @@
       </c>
     </row>
     <row r="58" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
       <c r="Q58">
         <v>0.58768200000000004</v>
       </c>
@@ -3450,8 +3428,6 @@
       </c>
     </row>
     <row r="59" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
       <c r="Q59">
         <v>0.54432199999999997</v>
       </c>
@@ -3475,8 +3451,6 @@
       </c>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
       <c r="Q60">
         <v>0.51415699999999998</v>
       </c>
@@ -3500,16 +3474,12 @@
       </c>
     </row>
     <row r="61" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
       <c r="U61" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="62" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="U62" s="25" t="s">
+      <c r="U62" s="22" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5444,8 +5414,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:2" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5460,7 +5430,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
+      <c r="A6" s="21"/>
       <c r="B6" t="s">
         <v>64</v>
       </c>
@@ -5472,7 +5442,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
+      <c r="A8" s="23"/>
       <c r="B8" t="s">
         <v>118</v>
       </c>
@@ -5525,20 +5495,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -6141,20 +6111,20 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="G43" s="23" t="s">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="G43" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">

</xml_diff>

<commit_message>
all hierarchical with correct saving, changed notebook so that correctly saved
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_final.xlsx
+++ b/models/evaluations/evaluation_prompts_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93450CB5-0C78-1A43-AAB2-F8C3E8A1FC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D628969B-88F2-674A-864D-49226BCF503B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="500" windowWidth="22860" windowHeight="15500" activeTab="1" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="295">
   <si>
     <t>prompt description</t>
   </si>
@@ -911,6 +911,78 @@
   </si>
   <si>
     <t>(0.356, 0.45)</t>
+  </si>
+  <si>
+    <t>(0.355, 0.526)</t>
+  </si>
+  <si>
+    <t>(0.272, 0.352)</t>
+  </si>
+  <si>
+    <t>(0.217, 0.3)</t>
+  </si>
+  <si>
+    <t>(0.273, 0.35)</t>
+  </si>
+  <si>
+    <t>(0.525, 0.622)</t>
+  </si>
+  <si>
+    <t>(0.464, 0.549)</t>
+  </si>
+  <si>
+    <t>(0.457, 0.546)</t>
+  </si>
+  <si>
+    <t>P2_HIERARCHY</t>
+  </si>
+  <si>
+    <t>P1_HIERARCHICAL</t>
+  </si>
+  <si>
+    <t>P2_HIERARCHICAL</t>
+  </si>
+  <si>
+    <t>(0.365, 0.535)</t>
+  </si>
+  <si>
+    <t>(0.273, 0.352)</t>
+  </si>
+  <si>
+    <t>(0.224, 0.308)</t>
+  </si>
+  <si>
+    <t>(0.275, 0.354)</t>
+  </si>
+  <si>
+    <t>(0.53, 0.629)</t>
+  </si>
+  <si>
+    <t>(0.461, 0.545)</t>
+  </si>
+  <si>
+    <t>(0.454, 0.543)</t>
+  </si>
+  <si>
+    <t>(0.463, 0.547)</t>
+  </si>
+  <si>
+    <t>(0.417, 0.586)</t>
+  </si>
+  <si>
+    <t>(0.307, 0.388)</t>
+  </si>
+  <si>
+    <t>(0.252, 0.338)</t>
+  </si>
+  <si>
+    <t>(0.561, 0.655)</t>
+  </si>
+  <si>
+    <t>(0.507, 0.592)</t>
+  </si>
+  <si>
+    <t>(0.495, 0.583)</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1154,6 +1226,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1496,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B1:BA62"/>
   <sheetViews>
-    <sheetView topLeftCell="F2" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:S2"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4885,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F016DC3-7647-EC40-938C-4348D53868B2}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="93" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35:S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6579,6 +6652,232 @@
       </c>
       <c r="AC26" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="L32" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="M32" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="N32" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="P32" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="R32" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="S32" s="34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="C33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D33">
+        <v>0.311</v>
+      </c>
+      <c r="E33" t="s">
+        <v>272</v>
+      </c>
+      <c r="F33">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G33" t="s">
+        <v>273</v>
+      </c>
+      <c r="H33">
+        <v>0.311</v>
+      </c>
+      <c r="I33" t="s">
+        <v>274</v>
+      </c>
+      <c r="L33">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="M33" t="s">
+        <v>275</v>
+      </c>
+      <c r="N33">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="O33" t="s">
+        <v>276</v>
+      </c>
+      <c r="P33">
+        <v>0.502</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>277</v>
+      </c>
+      <c r="R33">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="S33" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="C34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34">
+        <v>0.313</v>
+      </c>
+      <c r="E34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F34">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G34" t="s">
+        <v>283</v>
+      </c>
+      <c r="H34">
+        <v>0.313</v>
+      </c>
+      <c r="I34" t="s">
+        <v>284</v>
+      </c>
+      <c r="L34">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M34" t="s">
+        <v>285</v>
+      </c>
+      <c r="N34">
+        <v>0.504</v>
+      </c>
+      <c r="O34" t="s">
+        <v>286</v>
+      </c>
+      <c r="P34">
+        <v>0.499</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>287</v>
+      </c>
+      <c r="R34">
+        <v>0.504</v>
+      </c>
+      <c r="S34" t="s">
+        <v>288</v>
+      </c>
+      <c r="T34" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="C35" t="s">
+        <v>289</v>
+      </c>
+      <c r="D35">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="E35" t="s">
+        <v>290</v>
+      </c>
+      <c r="F35">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G35" t="s">
+        <v>291</v>
+      </c>
+      <c r="H35">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="I35" t="s">
+        <v>290</v>
+      </c>
+      <c r="L35">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="M35" t="s">
+        <v>292</v>
+      </c>
+      <c r="N35">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="O35" t="s">
+        <v>293</v>
+      </c>
+      <c r="P35">
+        <v>0.54</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>294</v>
+      </c>
+      <c r="R35">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="S35" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did all binary and hierarchical with confidence interval, saved correctly
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_final.xlsx
+++ b/models/evaluations/evaluation_prompts_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D628969B-88F2-674A-864D-49226BCF503B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98438313-6F5E-3B4D-8EC4-4A1223A628BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="500" windowWidth="22860" windowHeight="15500" activeTab="1" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="4120" yWindow="500" windowWidth="22860" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="312">
   <si>
     <t>prompt description</t>
   </si>
@@ -934,9 +934,6 @@
     <t>(0.457, 0.546)</t>
   </si>
   <si>
-    <t>P2_HIERARCHY</t>
-  </si>
-  <si>
     <t>P1_HIERARCHICAL</t>
   </si>
   <si>
@@ -983,6 +980,60 @@
   </si>
   <si>
     <t>(0.495, 0.583)</t>
+  </si>
+  <si>
+    <t>(0.699, 0.772)</t>
+  </si>
+  <si>
+    <t>(0.603, 0.684)</t>
+  </si>
+  <si>
+    <t>(0.603, 0.686)</t>
+  </si>
+  <si>
+    <t>gpt-4, P3_P2_HIERARCHICAL</t>
+  </si>
+  <si>
+    <t>(0.888, 0.94)</t>
+  </si>
+  <si>
+    <t>(0.897, 0.942)</t>
+  </si>
+  <si>
+    <t>(0.884, 0.938)</t>
+  </si>
+  <si>
+    <t>(0.883, 0.935)</t>
+  </si>
+  <si>
+    <t>(0.89, 0.936)</t>
+  </si>
+  <si>
+    <t>(0.875, 0.932)</t>
+  </si>
+  <si>
+    <t>(0.927, 0.964)</t>
+  </si>
+  <si>
+    <t>(0.923, 0.963)</t>
+  </si>
+  <si>
+    <t>(0.925, 0.963)</t>
+  </si>
+  <si>
+    <t>(0.923, 0.963</t>
+  </si>
+  <si>
+    <t>(0.968, 0.988)</t>
+  </si>
+  <si>
+    <t>(0.961, 0.987)</t>
+  </si>
+  <si>
+    <t>(0.962, 0.987)</t>
+  </si>
+  <si>
+    <t>P3, gpt-4</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1227,6 +1278,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1569,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B1:BA62"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScaleNormal="56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="56" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -4958,10 +5010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F016DC3-7647-EC40-938C-4348D53868B2}">
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="93" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35:S35"/>
+    <sheetView topLeftCell="A22" zoomScale="93" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6659,10 +6711,10 @@
         <v>84</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
@@ -6718,7 +6770,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
@@ -6771,7 +6823,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
@@ -6779,55 +6831,52 @@
         <v>0.45200000000000001</v>
       </c>
       <c r="C34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D34">
         <v>0.313</v>
       </c>
       <c r="E34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F34">
         <v>0.26500000000000001</v>
       </c>
       <c r="G34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H34">
         <v>0.313</v>
       </c>
       <c r="I34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L34">
         <v>0.58699999999999997</v>
       </c>
       <c r="M34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N34">
         <v>0.504</v>
       </c>
       <c r="O34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P34">
         <v>0.499</v>
       </c>
       <c r="Q34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R34">
         <v>0.504</v>
       </c>
       <c r="S34" t="s">
-        <v>288</v>
-      </c>
-      <c r="T34" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>7</v>
       </c>
@@ -6835,49 +6884,230 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="C35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D35">
         <v>0.34599999999999997</v>
       </c>
       <c r="E35" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F35">
         <v>0.29499999999999998</v>
       </c>
       <c r="G35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H35">
         <v>0.34599999999999997</v>
       </c>
       <c r="I35" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L35">
         <v>0.61699999999999999</v>
       </c>
       <c r="M35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N35">
         <v>0.55100000000000005</v>
       </c>
       <c r="O35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P35">
         <v>0.54</v>
       </c>
       <c r="Q35" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R35">
         <v>0.55100000000000005</v>
       </c>
       <c r="S35" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L36" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="M37" t="s">
+        <v>294</v>
+      </c>
+      <c r="N37">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="O37" t="s">
+        <v>295</v>
+      </c>
+      <c r="P37">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>296</v>
+      </c>
+      <c r="R37">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="S37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="C40" t="s">
+        <v>298</v>
+      </c>
+      <c r="D40">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="E40" t="s">
+        <v>299</v>
+      </c>
+      <c r="F40">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="G40" t="s">
+        <v>300</v>
+      </c>
+      <c r="H40">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="I40" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="C41" t="s">
+        <v>301</v>
+      </c>
+      <c r="D41">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="E41" t="s">
+        <v>302</v>
+      </c>
+      <c r="F41">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="G41" t="s">
+        <v>303</v>
+      </c>
+      <c r="H41">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="I41" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="C42" t="s">
+        <v>304</v>
+      </c>
+      <c r="D42">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="E42" t="s">
+        <v>305</v>
+      </c>
+      <c r="F42">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="G42" t="s">
+        <v>306</v>
+      </c>
+      <c r="H42">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="I42" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
+        <v>311</v>
+      </c>
+      <c r="B43">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="C43" t="s">
+        <v>308</v>
+      </c>
+      <c r="D43">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="E43" t="s">
+        <v>309</v>
+      </c>
+      <c r="F43">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G43" t="s">
+        <v>310</v>
+      </c>
+      <c r="H43">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I43" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to evaluate differenc ein CI's of unenriched vs enriched - seems to be difference which is not always the same, which could speak for GPT profiting from enrichment??
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts_final.xlsx
+++ b/models/evaluations/evaluation_prompts_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98438313-6F5E-3B4D-8EC4-4A1223A628BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A74B0D7-FEE3-E344-8E5E-824DB258B0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="500" windowWidth="22860" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="4120" yWindow="500" windowWidth="22860" windowHeight="15500" activeTab="1" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="327">
   <si>
     <t>prompt description</t>
   </si>
@@ -1034,6 +1034,51 @@
   </si>
   <si>
     <t>P3, gpt-4</t>
+  </si>
+  <si>
+    <t>0.23, 0.23</t>
+  </si>
+  <si>
+    <t>(0.308, 0.409)0.308</t>
+  </si>
+  <si>
+    <t>(0.321, 0.424)0.321</t>
+  </si>
+  <si>
+    <t>(0.308, 0.41)0.308</t>
+  </si>
+  <si>
+    <t>(0.33, 0.433)0.33</t>
+  </si>
+  <si>
+    <t>(0.297, 0.399)0.297</t>
+  </si>
+  <si>
+    <t>(0.307, 0.408)0.307</t>
+  </si>
+  <si>
+    <t>(0.359, 0.463)0.359</t>
+  </si>
+  <si>
+    <t>(0.424, 0.527)0.424</t>
+  </si>
+  <si>
+    <t>(0.149, 0.236)0.149</t>
+  </si>
+  <si>
+    <t>Delta under CI</t>
+  </si>
+  <si>
+    <t>Delta upper CI</t>
+  </si>
+  <si>
+    <t>Sum of Deltas</t>
+  </si>
+  <si>
+    <t>CI enriched</t>
+  </si>
+  <si>
+    <t>CI unenriched</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1255,6 +1300,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1279,6 +1325,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1621,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B1:BA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="56" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="75" zoomScaleNormal="56" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -1663,27 +1715,27 @@
       <c r="X1" t="s">
         <v>75</v>
       </c>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="23"/>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="24"/>
     </row>
     <row r="2" spans="2:53" x14ac:dyDescent="0.2">
       <c r="E2" s="1" t="s">
@@ -1715,27 +1767,27 @@
       <c r="AD2" s="20"/>
       <c r="AE2" s="20"/>
       <c r="AF2" s="5"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="26"/>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23"/>
-      <c r="AY2" s="24"/>
-      <c r="AZ2" s="24"/>
-      <c r="BA2" s="24"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="24"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="24"/>
+      <c r="AQ2" s="24"/>
+      <c r="AR2" s="24"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="23"/>
+      <c r="AU2" s="23"/>
+      <c r="AV2" s="24"/>
+      <c r="AW2" s="24"/>
+      <c r="AX2" s="24"/>
+      <c r="AY2" s="25"/>
+      <c r="AZ2" s="25"/>
+      <c r="BA2" s="25"/>
     </row>
     <row r="3" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -1803,27 +1855,27 @@
         <v>4</v>
       </c>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="23"/>
-      <c r="AI3" s="22"/>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="22"/>
-      <c r="AL3" s="23"/>
-      <c r="AM3" s="22"/>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="23"/>
-      <c r="AQ3" s="22"/>
-      <c r="AR3" s="23"/>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="22"/>
-      <c r="AU3" s="22"/>
-      <c r="AV3" s="23"/>
-      <c r="AW3" s="22"/>
-      <c r="AX3" s="23"/>
-      <c r="AY3" s="22"/>
-      <c r="AZ3" s="22"/>
-      <c r="BA3" s="22"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="24"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
     </row>
     <row r="4" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
@@ -1891,27 +1943,27 @@
         <v>0.39852399999999999</v>
       </c>
       <c r="AF4" s="2"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="23"/>
-      <c r="AL4" s="23"/>
-      <c r="AM4" s="23"/>
-      <c r="AN4" s="23"/>
-      <c r="AO4" s="23"/>
-      <c r="AP4" s="23"/>
-      <c r="AQ4" s="23"/>
-      <c r="AR4" s="23"/>
-      <c r="AS4" s="23"/>
-      <c r="AT4" s="23"/>
-      <c r="AU4" s="23"/>
-      <c r="AV4" s="23"/>
-      <c r="AW4" s="23"/>
-      <c r="AX4" s="23"/>
-      <c r="AY4" s="23"/>
-      <c r="AZ4" s="23"/>
-      <c r="BA4" s="23"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="28"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
+      <c r="AM4" s="24"/>
+      <c r="AN4" s="24"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="24"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="24"/>
+      <c r="AS4" s="24"/>
+      <c r="AT4" s="24"/>
+      <c r="AU4" s="24"/>
+      <c r="AV4" s="24"/>
+      <c r="AW4" s="24"/>
+      <c r="AX4" s="24"/>
+      <c r="AY4" s="24"/>
+      <c r="AZ4" s="24"/>
+      <c r="BA4" s="24"/>
     </row>
     <row r="5" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
@@ -1960,27 +2012,27 @@
         <v>6</v>
       </c>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="23"/>
-      <c r="AL5" s="23"/>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="23"/>
-      <c r="AO5" s="23"/>
-      <c r="AP5" s="23"/>
-      <c r="AQ5" s="23"/>
-      <c r="AR5" s="23"/>
-      <c r="AS5" s="23"/>
-      <c r="AT5" s="23"/>
-      <c r="AU5" s="23"/>
-      <c r="AV5" s="23"/>
-      <c r="AW5" s="23"/>
-      <c r="AX5" s="23"/>
-      <c r="AY5" s="23"/>
-      <c r="AZ5" s="23"/>
-      <c r="BA5" s="23"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="28"/>
+      <c r="AJ5" s="28"/>
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="24"/>
+      <c r="AM5" s="24"/>
+      <c r="AN5" s="24"/>
+      <c r="AO5" s="24"/>
+      <c r="AP5" s="24"/>
+      <c r="AQ5" s="24"/>
+      <c r="AR5" s="24"/>
+      <c r="AS5" s="24"/>
+      <c r="AT5" s="24"/>
+      <c r="AU5" s="24"/>
+      <c r="AV5" s="24"/>
+      <c r="AW5" s="24"/>
+      <c r="AX5" s="24"/>
+      <c r="AY5" s="24"/>
+      <c r="AZ5" s="24"/>
+      <c r="BA5" s="24"/>
     </row>
     <row r="6" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
@@ -2014,27 +2066,27 @@
       <c r="AA6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AG6" s="32"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="23"/>
-      <c r="AJ6" s="23"/>
-      <c r="AK6" s="25"/>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="25"/>
-      <c r="AR6" s="23"/>
-      <c r="AS6" s="23"/>
-      <c r="AT6" s="23"/>
-      <c r="AU6" s="23"/>
-      <c r="AV6" s="23"/>
-      <c r="AW6" s="25"/>
-      <c r="AX6" s="23"/>
-      <c r="AY6" s="23"/>
-      <c r="AZ6" s="23"/>
-      <c r="BA6" s="23"/>
+      <c r="AG6" s="33"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="24"/>
+      <c r="AK6" s="26"/>
+      <c r="AL6" s="24"/>
+      <c r="AM6" s="24"/>
+      <c r="AN6" s="24"/>
+      <c r="AO6" s="24"/>
+      <c r="AP6" s="24"/>
+      <c r="AQ6" s="26"/>
+      <c r="AR6" s="24"/>
+      <c r="AS6" s="24"/>
+      <c r="AT6" s="24"/>
+      <c r="AU6" s="24"/>
+      <c r="AV6" s="24"/>
+      <c r="AW6" s="26"/>
+      <c r="AX6" s="24"/>
+      <c r="AY6" s="24"/>
+      <c r="AZ6" s="24"/>
+      <c r="BA6" s="24"/>
     </row>
     <row r="7" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
@@ -2067,27 +2119,27 @@
       <c r="AA7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AG7" s="32"/>
-      <c r="AH7" s="23"/>
-      <c r="AI7" s="23"/>
-      <c r="AJ7" s="23"/>
-      <c r="AK7" s="25"/>
-      <c r="AL7" s="23"/>
-      <c r="AM7" s="23"/>
-      <c r="AN7" s="23"/>
-      <c r="AO7" s="23"/>
-      <c r="AP7" s="23"/>
-      <c r="AQ7" s="25"/>
-      <c r="AR7" s="23"/>
-      <c r="AS7" s="23"/>
-      <c r="AT7" s="23"/>
-      <c r="AU7" s="23"/>
-      <c r="AV7" s="23"/>
-      <c r="AW7" s="25"/>
-      <c r="AX7" s="23"/>
-      <c r="AY7" s="23"/>
-      <c r="AZ7" s="23"/>
-      <c r="BA7" s="23"/>
+      <c r="AG7" s="33"/>
+      <c r="AH7" s="24"/>
+      <c r="AI7" s="24"/>
+      <c r="AJ7" s="24"/>
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="24"/>
+      <c r="AM7" s="24"/>
+      <c r="AN7" s="24"/>
+      <c r="AO7" s="24"/>
+      <c r="AP7" s="24"/>
+      <c r="AQ7" s="26"/>
+      <c r="AR7" s="24"/>
+      <c r="AS7" s="24"/>
+      <c r="AT7" s="24"/>
+      <c r="AU7" s="24"/>
+      <c r="AV7" s="24"/>
+      <c r="AW7" s="26"/>
+      <c r="AX7" s="24"/>
+      <c r="AY7" s="24"/>
+      <c r="AZ7" s="24"/>
+      <c r="BA7" s="24"/>
     </row>
     <row r="8" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
@@ -2140,27 +2192,27 @@
         <v>8</v>
       </c>
       <c r="AF8" s="2"/>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="23"/>
-      <c r="AJ8" s="23"/>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="23"/>
-      <c r="AN8" s="23"/>
-      <c r="AO8" s="23"/>
-      <c r="AP8" s="23"/>
-      <c r="AQ8" s="23"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="23"/>
-      <c r="AT8" s="23"/>
-      <c r="AU8" s="23"/>
-      <c r="AV8" s="23"/>
-      <c r="AW8" s="23"/>
-      <c r="AX8" s="23"/>
-      <c r="AY8" s="23"/>
-      <c r="AZ8" s="23"/>
-      <c r="BA8" s="23"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="24"/>
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="24"/>
+      <c r="AL8" s="24"/>
+      <c r="AM8" s="24"/>
+      <c r="AN8" s="24"/>
+      <c r="AO8" s="24"/>
+      <c r="AP8" s="24"/>
+      <c r="AQ8" s="24"/>
+      <c r="AR8" s="24"/>
+      <c r="AS8" s="24"/>
+      <c r="AT8" s="24"/>
+      <c r="AU8" s="24"/>
+      <c r="AV8" s="24"/>
+      <c r="AW8" s="24"/>
+      <c r="AX8" s="24"/>
+      <c r="AY8" s="24"/>
+      <c r="AZ8" s="24"/>
+      <c r="BA8" s="24"/>
     </row>
     <row r="9" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
@@ -2213,27 +2265,27 @@
         <v>9</v>
       </c>
       <c r="AF9" s="2"/>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="23"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="23"/>
-      <c r="AO9" s="23"/>
-      <c r="AP9" s="23"/>
-      <c r="AQ9" s="23"/>
-      <c r="AR9" s="23"/>
-      <c r="AS9" s="23"/>
-      <c r="AT9" s="23"/>
-      <c r="AU9" s="23"/>
-      <c r="AV9" s="23"/>
-      <c r="AW9" s="23"/>
-      <c r="AX9" s="23"/>
-      <c r="AY9" s="23"/>
-      <c r="AZ9" s="23"/>
-      <c r="BA9" s="23"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="24"/>
+      <c r="AK9" s="24"/>
+      <c r="AL9" s="24"/>
+      <c r="AM9" s="24"/>
+      <c r="AN9" s="24"/>
+      <c r="AO9" s="24"/>
+      <c r="AP9" s="24"/>
+      <c r="AQ9" s="24"/>
+      <c r="AR9" s="24"/>
+      <c r="AS9" s="24"/>
+      <c r="AT9" s="24"/>
+      <c r="AU9" s="24"/>
+      <c r="AV9" s="24"/>
+      <c r="AW9" s="24"/>
+      <c r="AX9" s="24"/>
+      <c r="AY9" s="24"/>
+      <c r="AZ9" s="24"/>
+      <c r="BA9" s="24"/>
     </row>
     <row r="10" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
@@ -2285,27 +2337,27 @@
         <v>10</v>
       </c>
       <c r="AF10" s="2"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="23"/>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="23"/>
-      <c r="AK10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="23"/>
-      <c r="AO10" s="23"/>
-      <c r="AP10" s="23"/>
-      <c r="AQ10" s="23"/>
-      <c r="AR10" s="23"/>
-      <c r="AS10" s="23"/>
-      <c r="AT10" s="23"/>
-      <c r="AU10" s="23"/>
-      <c r="AV10" s="23"/>
-      <c r="AW10" s="23"/>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="23"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="24"/>
+      <c r="AJ10" s="24"/>
+      <c r="AK10" s="24"/>
+      <c r="AL10" s="24"/>
+      <c r="AM10" s="24"/>
+      <c r="AN10" s="24"/>
+      <c r="AO10" s="24"/>
+      <c r="AP10" s="24"/>
+      <c r="AQ10" s="24"/>
+      <c r="AR10" s="24"/>
+      <c r="AS10" s="24"/>
+      <c r="AT10" s="24"/>
+      <c r="AU10" s="24"/>
+      <c r="AV10" s="24"/>
+      <c r="AW10" s="24"/>
+      <c r="AX10" s="24"/>
+      <c r="AY10" s="24"/>
+      <c r="AZ10" s="24"/>
+      <c r="BA10" s="24"/>
     </row>
     <row r="11" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
@@ -2357,27 +2409,27 @@
       <c r="AA11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="23"/>
-      <c r="AI11" s="23"/>
-      <c r="AJ11" s="23"/>
-      <c r="AK11" s="23"/>
-      <c r="AL11" s="23"/>
-      <c r="AM11" s="23"/>
-      <c r="AN11" s="23"/>
-      <c r="AO11" s="23"/>
-      <c r="AP11" s="23"/>
-      <c r="AQ11" s="23"/>
-      <c r="AR11" s="23"/>
-      <c r="AS11" s="23"/>
-      <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
-      <c r="AV11" s="23"/>
-      <c r="AW11" s="23"/>
-      <c r="AX11" s="23"/>
-      <c r="AY11" s="23"/>
-      <c r="AZ11" s="23"/>
-      <c r="BA11" s="23"/>
+      <c r="AG11" s="28"/>
+      <c r="AH11" s="24"/>
+      <c r="AI11" s="24"/>
+      <c r="AJ11" s="24"/>
+      <c r="AK11" s="24"/>
+      <c r="AL11" s="24"/>
+      <c r="AM11" s="24"/>
+      <c r="AN11" s="24"/>
+      <c r="AO11" s="24"/>
+      <c r="AP11" s="24"/>
+      <c r="AQ11" s="24"/>
+      <c r="AR11" s="24"/>
+      <c r="AS11" s="24"/>
+      <c r="AT11" s="24"/>
+      <c r="AU11" s="24"/>
+      <c r="AV11" s="24"/>
+      <c r="AW11" s="24"/>
+      <c r="AX11" s="24"/>
+      <c r="AY11" s="24"/>
+      <c r="AZ11" s="24"/>
+      <c r="BA11" s="24"/>
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -2410,27 +2462,27 @@
       <c r="AA12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AG12" s="32"/>
-      <c r="AH12" s="23"/>
-      <c r="AI12" s="23"/>
-      <c r="AJ12" s="23"/>
-      <c r="AK12" s="25"/>
-      <c r="AL12" s="23"/>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="23"/>
-      <c r="AP12" s="23"/>
-      <c r="AQ12" s="25"/>
-      <c r="AR12" s="23"/>
-      <c r="AS12" s="23"/>
-      <c r="AT12" s="23"/>
-      <c r="AU12" s="23"/>
-      <c r="AV12" s="23"/>
-      <c r="AW12" s="25"/>
-      <c r="AX12" s="23"/>
-      <c r="AY12" s="23"/>
-      <c r="AZ12" s="23"/>
-      <c r="BA12" s="23"/>
+      <c r="AG12" s="33"/>
+      <c r="AH12" s="24"/>
+      <c r="AI12" s="24"/>
+      <c r="AJ12" s="24"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="24"/>
+      <c r="AM12" s="24"/>
+      <c r="AN12" s="24"/>
+      <c r="AO12" s="24"/>
+      <c r="AP12" s="24"/>
+      <c r="AQ12" s="26"/>
+      <c r="AR12" s="24"/>
+      <c r="AS12" s="24"/>
+      <c r="AT12" s="24"/>
+      <c r="AU12" s="24"/>
+      <c r="AV12" s="24"/>
+      <c r="AW12" s="26"/>
+      <c r="AX12" s="24"/>
+      <c r="AY12" s="24"/>
+      <c r="AZ12" s="24"/>
+      <c r="BA12" s="24"/>
     </row>
     <row r="13" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
@@ -2502,27 +2554,27 @@
         <v>0.556975</v>
       </c>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="23"/>
-      <c r="AI13" s="23"/>
-      <c r="AJ13" s="23"/>
-      <c r="AK13" s="23"/>
-      <c r="AL13" s="23"/>
-      <c r="AM13" s="23"/>
-      <c r="AN13" s="23"/>
-      <c r="AO13" s="23"/>
-      <c r="AP13" s="23"/>
-      <c r="AQ13" s="23"/>
-      <c r="AR13" s="23"/>
-      <c r="AS13" s="23"/>
-      <c r="AT13" s="23"/>
-      <c r="AU13" s="23"/>
-      <c r="AV13" s="23"/>
-      <c r="AW13" s="23"/>
-      <c r="AX13" s="23"/>
-      <c r="AY13" s="23"/>
-      <c r="AZ13" s="23"/>
-      <c r="BA13" s="23"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="24"/>
+      <c r="AI13" s="24"/>
+      <c r="AJ13" s="24"/>
+      <c r="AK13" s="24"/>
+      <c r="AL13" s="24"/>
+      <c r="AM13" s="24"/>
+      <c r="AN13" s="24"/>
+      <c r="AO13" s="24"/>
+      <c r="AP13" s="24"/>
+      <c r="AQ13" s="24"/>
+      <c r="AR13" s="24"/>
+      <c r="AS13" s="24"/>
+      <c r="AT13" s="24"/>
+      <c r="AU13" s="24"/>
+      <c r="AV13" s="24"/>
+      <c r="AW13" s="24"/>
+      <c r="AX13" s="24"/>
+      <c r="AY13" s="24"/>
+      <c r="AZ13" s="24"/>
+      <c r="BA13" s="24"/>
     </row>
     <row r="14" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
@@ -2573,27 +2625,27 @@
       <c r="AA14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="23"/>
-      <c r="AI14" s="23"/>
-      <c r="AJ14" s="23"/>
-      <c r="AK14" s="23"/>
-      <c r="AL14" s="23"/>
-      <c r="AM14" s="23"/>
-      <c r="AN14" s="23"/>
-      <c r="AO14" s="23"/>
-      <c r="AP14" s="23"/>
-      <c r="AQ14" s="23"/>
-      <c r="AR14" s="23"/>
-      <c r="AS14" s="23"/>
-      <c r="AT14" s="23"/>
-      <c r="AU14" s="23"/>
-      <c r="AV14" s="23"/>
-      <c r="AW14" s="23"/>
-      <c r="AX14" s="23"/>
-      <c r="AY14" s="23"/>
-      <c r="AZ14" s="23"/>
-      <c r="BA14" s="23"/>
+      <c r="AG14" s="28"/>
+      <c r="AH14" s="24"/>
+      <c r="AI14" s="24"/>
+      <c r="AJ14" s="24"/>
+      <c r="AK14" s="24"/>
+      <c r="AL14" s="24"/>
+      <c r="AM14" s="24"/>
+      <c r="AN14" s="24"/>
+      <c r="AO14" s="24"/>
+      <c r="AP14" s="24"/>
+      <c r="AQ14" s="24"/>
+      <c r="AR14" s="24"/>
+      <c r="AS14" s="24"/>
+      <c r="AT14" s="24"/>
+      <c r="AU14" s="24"/>
+      <c r="AV14" s="24"/>
+      <c r="AW14" s="24"/>
+      <c r="AX14" s="24"/>
+      <c r="AY14" s="24"/>
+      <c r="AZ14" s="24"/>
+      <c r="BA14" s="24"/>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
@@ -2660,27 +2712,27 @@
       <c r="AE15">
         <v>0.55549099999999996</v>
       </c>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="23"/>
-      <c r="AI15" s="23"/>
-      <c r="AJ15" s="23"/>
-      <c r="AK15" s="23"/>
-      <c r="AL15" s="23"/>
-      <c r="AM15" s="23"/>
-      <c r="AN15" s="23"/>
-      <c r="AO15" s="23"/>
-      <c r="AP15" s="23"/>
-      <c r="AQ15" s="23"/>
-      <c r="AR15" s="23"/>
-      <c r="AS15" s="23"/>
-      <c r="AT15" s="23"/>
-      <c r="AU15" s="23"/>
-      <c r="AV15" s="23"/>
-      <c r="AW15" s="23"/>
-      <c r="AX15" s="23"/>
-      <c r="AY15" s="23"/>
-      <c r="AZ15" s="23"/>
-      <c r="BA15" s="23"/>
+      <c r="AG15" s="28"/>
+      <c r="AH15" s="24"/>
+      <c r="AI15" s="24"/>
+      <c r="AJ15" s="24"/>
+      <c r="AK15" s="24"/>
+      <c r="AL15" s="24"/>
+      <c r="AM15" s="24"/>
+      <c r="AN15" s="24"/>
+      <c r="AO15" s="24"/>
+      <c r="AP15" s="24"/>
+      <c r="AQ15" s="24"/>
+      <c r="AR15" s="24"/>
+      <c r="AS15" s="24"/>
+      <c r="AT15" s="24"/>
+      <c r="AU15" s="24"/>
+      <c r="AV15" s="24"/>
+      <c r="AW15" s="24"/>
+      <c r="AX15" s="24"/>
+      <c r="AY15" s="24"/>
+      <c r="AZ15" s="24"/>
+      <c r="BA15" s="24"/>
     </row>
     <row r="16" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
@@ -2748,27 +2800,27 @@
       <c r="AE16">
         <v>0.57348399999999999</v>
       </c>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="23"/>
-      <c r="AI16" s="23"/>
-      <c r="AJ16" s="23"/>
-      <c r="AK16" s="23"/>
-      <c r="AL16" s="23"/>
-      <c r="AM16" s="23"/>
-      <c r="AN16" s="23"/>
-      <c r="AO16" s="23"/>
-      <c r="AP16" s="23"/>
-      <c r="AQ16" s="23"/>
-      <c r="AR16" s="23"/>
-      <c r="AS16" s="23"/>
-      <c r="AT16" s="23"/>
-      <c r="AU16" s="23"/>
-      <c r="AV16" s="23"/>
-      <c r="AW16" s="23"/>
-      <c r="AX16" s="23"/>
-      <c r="AY16" s="23"/>
-      <c r="AZ16" s="23"/>
-      <c r="BA16" s="23"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="24"/>
+      <c r="AI16" s="24"/>
+      <c r="AJ16" s="24"/>
+      <c r="AK16" s="24"/>
+      <c r="AL16" s="24"/>
+      <c r="AM16" s="24"/>
+      <c r="AN16" s="24"/>
+      <c r="AO16" s="24"/>
+      <c r="AP16" s="24"/>
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="24"/>
+      <c r="AS16" s="24"/>
+      <c r="AT16" s="24"/>
+      <c r="AU16" s="24"/>
+      <c r="AV16" s="24"/>
+      <c r="AW16" s="24"/>
+      <c r="AX16" s="24"/>
+      <c r="AY16" s="24"/>
+      <c r="AZ16" s="24"/>
+      <c r="BA16" s="24"/>
     </row>
     <row r="17" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
@@ -2835,27 +2887,27 @@
       <c r="AE17">
         <v>0.34958600000000001</v>
       </c>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="23"/>
-      <c r="AI17" s="23"/>
-      <c r="AJ17" s="23"/>
-      <c r="AK17" s="23"/>
-      <c r="AL17" s="23"/>
-      <c r="AM17" s="23"/>
-      <c r="AN17" s="23"/>
-      <c r="AO17" s="23"/>
-      <c r="AP17" s="23"/>
-      <c r="AQ17" s="23"/>
-      <c r="AR17" s="23"/>
-      <c r="AS17" s="23"/>
-      <c r="AT17" s="23"/>
-      <c r="AU17" s="23"/>
-      <c r="AV17" s="23"/>
-      <c r="AW17" s="23"/>
-      <c r="AX17" s="23"/>
-      <c r="AY17" s="23"/>
-      <c r="AZ17" s="23"/>
-      <c r="BA17" s="23"/>
+      <c r="AG17" s="28"/>
+      <c r="AH17" s="24"/>
+      <c r="AI17" s="24"/>
+      <c r="AJ17" s="24"/>
+      <c r="AK17" s="24"/>
+      <c r="AL17" s="24"/>
+      <c r="AM17" s="24"/>
+      <c r="AN17" s="24"/>
+      <c r="AO17" s="24"/>
+      <c r="AP17" s="24"/>
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="24"/>
+      <c r="AS17" s="24"/>
+      <c r="AT17" s="24"/>
+      <c r="AU17" s="24"/>
+      <c r="AV17" s="24"/>
+      <c r="AW17" s="24"/>
+      <c r="AX17" s="24"/>
+      <c r="AY17" s="24"/>
+      <c r="AZ17" s="24"/>
+      <c r="BA17" s="24"/>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
@@ -2888,27 +2940,27 @@
       <c r="AA18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AG18" s="32"/>
-      <c r="AH18" s="23"/>
-      <c r="AI18" s="23"/>
-      <c r="AJ18" s="23"/>
-      <c r="AK18" s="25"/>
-      <c r="AL18" s="23"/>
-      <c r="AM18" s="23"/>
-      <c r="AN18" s="23"/>
-      <c r="AO18" s="23"/>
-      <c r="AP18" s="23"/>
-      <c r="AQ18" s="25"/>
-      <c r="AR18" s="23"/>
-      <c r="AS18" s="23"/>
-      <c r="AT18" s="23"/>
-      <c r="AU18" s="23"/>
-      <c r="AV18" s="23"/>
-      <c r="AW18" s="25"/>
-      <c r="AX18" s="23"/>
-      <c r="AY18" s="23"/>
-      <c r="AZ18" s="23"/>
-      <c r="BA18" s="23"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="24"/>
+      <c r="AI18" s="24"/>
+      <c r="AJ18" s="24"/>
+      <c r="AK18" s="26"/>
+      <c r="AL18" s="24"/>
+      <c r="AM18" s="24"/>
+      <c r="AN18" s="24"/>
+      <c r="AO18" s="24"/>
+      <c r="AP18" s="24"/>
+      <c r="AQ18" s="26"/>
+      <c r="AR18" s="24"/>
+      <c r="AS18" s="24"/>
+      <c r="AT18" s="24"/>
+      <c r="AU18" s="24"/>
+      <c r="AV18" s="24"/>
+      <c r="AW18" s="26"/>
+      <c r="AX18" s="24"/>
+      <c r="AY18" s="24"/>
+      <c r="AZ18" s="24"/>
+      <c r="BA18" s="24"/>
     </row>
     <row r="19" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
@@ -2959,27 +3011,27 @@
       <c r="AA19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AG19" s="27"/>
-      <c r="AH19" s="23"/>
-      <c r="AI19" s="23"/>
-      <c r="AJ19" s="23"/>
-      <c r="AK19" s="23"/>
-      <c r="AL19" s="23"/>
-      <c r="AM19" s="23"/>
-      <c r="AN19" s="23"/>
-      <c r="AO19" s="23"/>
-      <c r="AP19" s="23"/>
-      <c r="AQ19" s="23"/>
-      <c r="AR19" s="23"/>
-      <c r="AS19" s="23"/>
-      <c r="AT19" s="23"/>
-      <c r="AU19" s="23"/>
-      <c r="AV19" s="23"/>
-      <c r="AW19" s="23"/>
-      <c r="AX19" s="23"/>
-      <c r="AY19" s="23"/>
-      <c r="AZ19" s="23"/>
-      <c r="BA19" s="23"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="24"/>
+      <c r="AI19" s="24"/>
+      <c r="AJ19" s="24"/>
+      <c r="AK19" s="24"/>
+      <c r="AL19" s="24"/>
+      <c r="AM19" s="24"/>
+      <c r="AN19" s="24"/>
+      <c r="AO19" s="24"/>
+      <c r="AP19" s="24"/>
+      <c r="AQ19" s="24"/>
+      <c r="AR19" s="24"/>
+      <c r="AS19" s="24"/>
+      <c r="AT19" s="24"/>
+      <c r="AU19" s="24"/>
+      <c r="AV19" s="24"/>
+      <c r="AW19" s="24"/>
+      <c r="AX19" s="24"/>
+      <c r="AY19" s="24"/>
+      <c r="AZ19" s="24"/>
+      <c r="BA19" s="24"/>
     </row>
     <row r="20" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
@@ -3030,27 +3082,27 @@
       <c r="AA20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AG20" s="27"/>
-      <c r="AH20" s="23"/>
-      <c r="AI20" s="23"/>
-      <c r="AJ20" s="23"/>
-      <c r="AK20" s="23"/>
-      <c r="AL20" s="23"/>
-      <c r="AM20" s="23"/>
-      <c r="AN20" s="23"/>
-      <c r="AO20" s="23"/>
-      <c r="AP20" s="23"/>
-      <c r="AQ20" s="23"/>
-      <c r="AR20" s="23"/>
-      <c r="AS20" s="23"/>
-      <c r="AT20" s="23"/>
-      <c r="AU20" s="23"/>
-      <c r="AV20" s="23"/>
-      <c r="AW20" s="23"/>
-      <c r="AX20" s="23"/>
-      <c r="AY20" s="23"/>
-      <c r="AZ20" s="23"/>
-      <c r="BA20" s="23"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="24"/>
+      <c r="AI20" s="24"/>
+      <c r="AJ20" s="24"/>
+      <c r="AK20" s="24"/>
+      <c r="AL20" s="24"/>
+      <c r="AM20" s="24"/>
+      <c r="AN20" s="24"/>
+      <c r="AO20" s="24"/>
+      <c r="AP20" s="24"/>
+      <c r="AQ20" s="24"/>
+      <c r="AR20" s="24"/>
+      <c r="AS20" s="24"/>
+      <c r="AT20" s="24"/>
+      <c r="AU20" s="24"/>
+      <c r="AV20" s="24"/>
+      <c r="AW20" s="24"/>
+      <c r="AX20" s="24"/>
+      <c r="AY20" s="24"/>
+      <c r="AZ20" s="24"/>
+      <c r="BA20" s="24"/>
     </row>
     <row r="21" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
@@ -3098,27 +3150,27 @@
       <c r="AA21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AG21" s="27"/>
-      <c r="AH21" s="23"/>
-      <c r="AI21" s="23"/>
-      <c r="AJ21" s="23"/>
-      <c r="AK21" s="23"/>
-      <c r="AL21" s="23"/>
-      <c r="AM21" s="23"/>
-      <c r="AN21" s="23"/>
-      <c r="AO21" s="23"/>
-      <c r="AP21" s="23"/>
-      <c r="AQ21" s="23"/>
-      <c r="AR21" s="23"/>
-      <c r="AS21" s="23"/>
-      <c r="AT21" s="23"/>
-      <c r="AU21" s="23"/>
-      <c r="AV21" s="23"/>
-      <c r="AW21" s="23"/>
-      <c r="AX21" s="23"/>
-      <c r="AY21" s="23"/>
-      <c r="AZ21" s="23"/>
-      <c r="BA21" s="23"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="24"/>
+      <c r="AI21" s="24"/>
+      <c r="AJ21" s="24"/>
+      <c r="AK21" s="24"/>
+      <c r="AL21" s="24"/>
+      <c r="AM21" s="24"/>
+      <c r="AN21" s="24"/>
+      <c r="AO21" s="24"/>
+      <c r="AP21" s="24"/>
+      <c r="AQ21" s="24"/>
+      <c r="AR21" s="24"/>
+      <c r="AS21" s="24"/>
+      <c r="AT21" s="24"/>
+      <c r="AU21" s="24"/>
+      <c r="AV21" s="24"/>
+      <c r="AW21" s="24"/>
+      <c r="AX21" s="24"/>
+      <c r="AY21" s="24"/>
+      <c r="AZ21" s="24"/>
+      <c r="BA21" s="24"/>
     </row>
     <row r="22" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
@@ -3166,27 +3218,27 @@
       <c r="AA22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AG22" s="27"/>
-      <c r="AH22" s="23"/>
-      <c r="AI22" s="23"/>
-      <c r="AJ22" s="23"/>
-      <c r="AK22" s="23"/>
-      <c r="AL22" s="23"/>
-      <c r="AM22" s="23"/>
-      <c r="AN22" s="23"/>
-      <c r="AO22" s="23"/>
-      <c r="AP22" s="23"/>
-      <c r="AQ22" s="23"/>
-      <c r="AR22" s="23"/>
-      <c r="AS22" s="23"/>
-      <c r="AT22" s="23"/>
-      <c r="AU22" s="23"/>
-      <c r="AV22" s="23"/>
-      <c r="AW22" s="23"/>
-      <c r="AX22" s="23"/>
-      <c r="AY22" s="23"/>
-      <c r="AZ22" s="23"/>
-      <c r="BA22" s="23"/>
+      <c r="AG22" s="28"/>
+      <c r="AH22" s="24"/>
+      <c r="AI22" s="24"/>
+      <c r="AJ22" s="24"/>
+      <c r="AK22" s="24"/>
+      <c r="AL22" s="24"/>
+      <c r="AM22" s="24"/>
+      <c r="AN22" s="24"/>
+      <c r="AO22" s="24"/>
+      <c r="AP22" s="24"/>
+      <c r="AQ22" s="24"/>
+      <c r="AR22" s="24"/>
+      <c r="AS22" s="24"/>
+      <c r="AT22" s="24"/>
+      <c r="AU22" s="24"/>
+      <c r="AV22" s="24"/>
+      <c r="AW22" s="24"/>
+      <c r="AX22" s="24"/>
+      <c r="AY22" s="24"/>
+      <c r="AZ22" s="24"/>
+      <c r="BA22" s="24"/>
     </row>
     <row r="23" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
@@ -3237,27 +3289,27 @@
       <c r="AA23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AG23" s="27"/>
-      <c r="AH23" s="23"/>
-      <c r="AI23" s="23"/>
-      <c r="AJ23" s="23"/>
-      <c r="AK23" s="23"/>
-      <c r="AL23" s="23"/>
-      <c r="AM23" s="23"/>
-      <c r="AN23" s="23"/>
-      <c r="AO23" s="23"/>
-      <c r="AP23" s="23"/>
-      <c r="AQ23" s="23"/>
-      <c r="AR23" s="23"/>
-      <c r="AS23" s="23"/>
-      <c r="AT23" s="23"/>
-      <c r="AU23" s="23"/>
-      <c r="AV23" s="23"/>
-      <c r="AW23" s="23"/>
-      <c r="AX23" s="23"/>
-      <c r="AY23" s="23"/>
-      <c r="AZ23" s="23"/>
-      <c r="BA23" s="23"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="24"/>
+      <c r="AI23" s="24"/>
+      <c r="AJ23" s="24"/>
+      <c r="AK23" s="24"/>
+      <c r="AL23" s="24"/>
+      <c r="AM23" s="24"/>
+      <c r="AN23" s="24"/>
+      <c r="AO23" s="24"/>
+      <c r="AP23" s="24"/>
+      <c r="AQ23" s="24"/>
+      <c r="AR23" s="24"/>
+      <c r="AS23" s="24"/>
+      <c r="AT23" s="24"/>
+      <c r="AU23" s="24"/>
+      <c r="AV23" s="24"/>
+      <c r="AW23" s="24"/>
+      <c r="AX23" s="24"/>
+      <c r="AY23" s="24"/>
+      <c r="AZ23" s="24"/>
+      <c r="BA23" s="24"/>
     </row>
     <row r="24" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
@@ -3308,27 +3360,27 @@
       <c r="AA24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AG24" s="27"/>
-      <c r="AH24" s="23"/>
-      <c r="AI24" s="23"/>
-      <c r="AJ24" s="23"/>
-      <c r="AK24" s="23"/>
-      <c r="AL24" s="23"/>
-      <c r="AM24" s="23"/>
-      <c r="AN24" s="23"/>
-      <c r="AO24" s="23"/>
-      <c r="AP24" s="23"/>
-      <c r="AQ24" s="23"/>
-      <c r="AR24" s="23"/>
-      <c r="AS24" s="23"/>
-      <c r="AT24" s="23"/>
-      <c r="AU24" s="23"/>
-      <c r="AV24" s="23"/>
-      <c r="AW24" s="23"/>
-      <c r="AX24" s="23"/>
-      <c r="AY24" s="23"/>
-      <c r="AZ24" s="23"/>
-      <c r="BA24" s="23"/>
+      <c r="AG24" s="28"/>
+      <c r="AH24" s="24"/>
+      <c r="AI24" s="24"/>
+      <c r="AJ24" s="24"/>
+      <c r="AK24" s="24"/>
+      <c r="AL24" s="24"/>
+      <c r="AM24" s="24"/>
+      <c r="AN24" s="24"/>
+      <c r="AO24" s="24"/>
+      <c r="AP24" s="24"/>
+      <c r="AQ24" s="24"/>
+      <c r="AR24" s="24"/>
+      <c r="AS24" s="24"/>
+      <c r="AT24" s="24"/>
+      <c r="AU24" s="24"/>
+      <c r="AV24" s="24"/>
+      <c r="AW24" s="24"/>
+      <c r="AX24" s="24"/>
+      <c r="AY24" s="24"/>
+      <c r="AZ24" s="24"/>
+      <c r="BA24" s="24"/>
     </row>
     <row r="25" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
@@ -3399,27 +3451,27 @@
       <c r="AE25">
         <v>0.560608</v>
       </c>
-      <c r="AG25" s="27"/>
-      <c r="AH25" s="23"/>
-      <c r="AI25" s="23"/>
-      <c r="AJ25" s="23"/>
-      <c r="AK25" s="23"/>
-      <c r="AL25" s="23"/>
-      <c r="AM25" s="23"/>
-      <c r="AN25" s="23"/>
-      <c r="AO25" s="23"/>
-      <c r="AP25" s="23"/>
-      <c r="AQ25" s="23"/>
-      <c r="AR25" s="23"/>
-      <c r="AS25" s="23"/>
-      <c r="AT25" s="23"/>
-      <c r="AU25" s="23"/>
-      <c r="AV25" s="23"/>
-      <c r="AW25" s="23"/>
-      <c r="AX25" s="23"/>
-      <c r="AY25" s="23"/>
-      <c r="AZ25" s="23"/>
-      <c r="BA25" s="23"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="24"/>
+      <c r="AI25" s="24"/>
+      <c r="AJ25" s="24"/>
+      <c r="AK25" s="24"/>
+      <c r="AL25" s="24"/>
+      <c r="AM25" s="24"/>
+      <c r="AN25" s="24"/>
+      <c r="AO25" s="24"/>
+      <c r="AP25" s="24"/>
+      <c r="AQ25" s="24"/>
+      <c r="AR25" s="24"/>
+      <c r="AS25" s="24"/>
+      <c r="AT25" s="24"/>
+      <c r="AU25" s="24"/>
+      <c r="AV25" s="24"/>
+      <c r="AW25" s="24"/>
+      <c r="AX25" s="24"/>
+      <c r="AY25" s="24"/>
+      <c r="AZ25" s="24"/>
+      <c r="BA25" s="24"/>
     </row>
     <row r="26" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
@@ -3490,27 +3542,27 @@
       <c r="AE26">
         <v>0.57139099999999998</v>
       </c>
-      <c r="AG26" s="27"/>
-      <c r="AH26" s="23"/>
-      <c r="AI26" s="23"/>
-      <c r="AJ26" s="23"/>
-      <c r="AK26" s="23"/>
-      <c r="AL26" s="23"/>
-      <c r="AM26" s="23"/>
-      <c r="AN26" s="23"/>
-      <c r="AO26" s="23"/>
-      <c r="AP26" s="23"/>
-      <c r="AQ26" s="23"/>
-      <c r="AR26" s="23"/>
-      <c r="AS26" s="23"/>
-      <c r="AT26" s="23"/>
-      <c r="AU26" s="23"/>
-      <c r="AV26" s="23"/>
-      <c r="AW26" s="23"/>
-      <c r="AX26" s="23"/>
-      <c r="AY26" s="23"/>
-      <c r="AZ26" s="23"/>
-      <c r="BA26" s="23"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="24"/>
+      <c r="AI26" s="24"/>
+      <c r="AJ26" s="24"/>
+      <c r="AK26" s="24"/>
+      <c r="AL26" s="24"/>
+      <c r="AM26" s="24"/>
+      <c r="AN26" s="24"/>
+      <c r="AO26" s="24"/>
+      <c r="AP26" s="24"/>
+      <c r="AQ26" s="24"/>
+      <c r="AR26" s="24"/>
+      <c r="AS26" s="24"/>
+      <c r="AT26" s="24"/>
+      <c r="AU26" s="24"/>
+      <c r="AV26" s="24"/>
+      <c r="AW26" s="24"/>
+      <c r="AX26" s="24"/>
+      <c r="AY26" s="24"/>
+      <c r="AZ26" s="24"/>
+      <c r="BA26" s="24"/>
     </row>
     <row r="27" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
@@ -3561,27 +3613,27 @@
       <c r="AA27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AG27" s="27"/>
-      <c r="AH27" s="23"/>
-      <c r="AI27" s="23"/>
-      <c r="AJ27" s="23"/>
-      <c r="AK27" s="23"/>
-      <c r="AL27" s="23"/>
-      <c r="AM27" s="23"/>
-      <c r="AN27" s="23"/>
-      <c r="AO27" s="23"/>
-      <c r="AP27" s="23"/>
-      <c r="AQ27" s="23"/>
-      <c r="AR27" s="23"/>
-      <c r="AS27" s="23"/>
-      <c r="AT27" s="23"/>
-      <c r="AU27" s="23"/>
-      <c r="AV27" s="23"/>
-      <c r="AW27" s="23"/>
-      <c r="AX27" s="23"/>
-      <c r="AY27" s="23"/>
-      <c r="AZ27" s="23"/>
-      <c r="BA27" s="23"/>
+      <c r="AG27" s="28"/>
+      <c r="AH27" s="24"/>
+      <c r="AI27" s="24"/>
+      <c r="AJ27" s="24"/>
+      <c r="AK27" s="24"/>
+      <c r="AL27" s="24"/>
+      <c r="AM27" s="24"/>
+      <c r="AN27" s="24"/>
+      <c r="AO27" s="24"/>
+      <c r="AP27" s="24"/>
+      <c r="AQ27" s="24"/>
+      <c r="AR27" s="24"/>
+      <c r="AS27" s="24"/>
+      <c r="AT27" s="24"/>
+      <c r="AU27" s="24"/>
+      <c r="AV27" s="24"/>
+      <c r="AW27" s="24"/>
+      <c r="AX27" s="24"/>
+      <c r="AY27" s="24"/>
+      <c r="AZ27" s="24"/>
+      <c r="BA27" s="24"/>
     </row>
     <row r="28" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
@@ -3629,27 +3681,27 @@
       <c r="AA28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AG28" s="27"/>
-      <c r="AH28" s="23"/>
-      <c r="AI28" s="23"/>
-      <c r="AJ28" s="23"/>
-      <c r="AK28" s="23"/>
-      <c r="AL28" s="23"/>
-      <c r="AM28" s="23"/>
-      <c r="AN28" s="23"/>
-      <c r="AO28" s="23"/>
-      <c r="AP28" s="23"/>
-      <c r="AQ28" s="23"/>
-      <c r="AR28" s="23"/>
-      <c r="AS28" s="23"/>
-      <c r="AT28" s="23"/>
-      <c r="AU28" s="23"/>
-      <c r="AV28" s="23"/>
-      <c r="AW28" s="23"/>
-      <c r="AX28" s="23"/>
-      <c r="AY28" s="23"/>
-      <c r="AZ28" s="23"/>
-      <c r="BA28" s="23"/>
+      <c r="AG28" s="28"/>
+      <c r="AH28" s="24"/>
+      <c r="AI28" s="24"/>
+      <c r="AJ28" s="24"/>
+      <c r="AK28" s="24"/>
+      <c r="AL28" s="24"/>
+      <c r="AM28" s="24"/>
+      <c r="AN28" s="24"/>
+      <c r="AO28" s="24"/>
+      <c r="AP28" s="24"/>
+      <c r="AQ28" s="24"/>
+      <c r="AR28" s="24"/>
+      <c r="AS28" s="24"/>
+      <c r="AT28" s="24"/>
+      <c r="AU28" s="24"/>
+      <c r="AV28" s="24"/>
+      <c r="AW28" s="24"/>
+      <c r="AX28" s="24"/>
+      <c r="AY28" s="24"/>
+      <c r="AZ28" s="24"/>
+      <c r="BA28" s="24"/>
     </row>
     <row r="29" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
@@ -3694,27 +3746,27 @@
       <c r="U29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="23"/>
-      <c r="AI29" s="23"/>
-      <c r="AJ29" s="23"/>
-      <c r="AK29" s="23"/>
-      <c r="AL29" s="23"/>
-      <c r="AM29" s="23"/>
-      <c r="AN29" s="23"/>
-      <c r="AO29" s="23"/>
-      <c r="AP29" s="23"/>
-      <c r="AQ29" s="23"/>
-      <c r="AR29" s="23"/>
-      <c r="AS29" s="23"/>
-      <c r="AT29" s="23"/>
-      <c r="AU29" s="23"/>
-      <c r="AV29" s="23"/>
-      <c r="AW29" s="23"/>
-      <c r="AX29" s="23"/>
-      <c r="AY29" s="23"/>
-      <c r="AZ29" s="23"/>
-      <c r="BA29" s="23"/>
+      <c r="AG29" s="28"/>
+      <c r="AH29" s="24"/>
+      <c r="AI29" s="24"/>
+      <c r="AJ29" s="24"/>
+      <c r="AK29" s="24"/>
+      <c r="AL29" s="24"/>
+      <c r="AM29" s="24"/>
+      <c r="AN29" s="24"/>
+      <c r="AO29" s="24"/>
+      <c r="AP29" s="24"/>
+      <c r="AQ29" s="24"/>
+      <c r="AR29" s="24"/>
+      <c r="AS29" s="24"/>
+      <c r="AT29" s="24"/>
+      <c r="AU29" s="24"/>
+      <c r="AV29" s="24"/>
+      <c r="AW29" s="24"/>
+      <c r="AX29" s="24"/>
+      <c r="AY29" s="24"/>
+      <c r="AZ29" s="24"/>
+      <c r="BA29" s="24"/>
     </row>
     <row r="30" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
@@ -3769,27 +3821,27 @@
       <c r="Y30">
         <v>0.56293199999999999</v>
       </c>
-      <c r="AG30" s="23"/>
-      <c r="AH30" s="23"/>
-      <c r="AI30" s="23"/>
-      <c r="AJ30" s="23"/>
-      <c r="AK30" s="23"/>
-      <c r="AL30" s="23"/>
-      <c r="AM30" s="23"/>
-      <c r="AN30" s="23"/>
-      <c r="AO30" s="23"/>
-      <c r="AP30" s="23"/>
-      <c r="AQ30" s="23"/>
-      <c r="AR30" s="23"/>
-      <c r="AS30" s="23"/>
-      <c r="AT30" s="23"/>
-      <c r="AU30" s="23"/>
-      <c r="AV30" s="23"/>
-      <c r="AW30" s="23"/>
-      <c r="AX30" s="23"/>
-      <c r="AY30" s="23"/>
-      <c r="AZ30" s="23"/>
-      <c r="BA30" s="23"/>
+      <c r="AG30" s="24"/>
+      <c r="AH30" s="24"/>
+      <c r="AI30" s="24"/>
+      <c r="AJ30" s="24"/>
+      <c r="AK30" s="24"/>
+      <c r="AL30" s="24"/>
+      <c r="AM30" s="24"/>
+      <c r="AN30" s="24"/>
+      <c r="AO30" s="24"/>
+      <c r="AP30" s="24"/>
+      <c r="AQ30" s="24"/>
+      <c r="AR30" s="24"/>
+      <c r="AS30" s="24"/>
+      <c r="AT30" s="24"/>
+      <c r="AU30" s="24"/>
+      <c r="AV30" s="24"/>
+      <c r="AW30" s="24"/>
+      <c r="AX30" s="24"/>
+      <c r="AY30" s="24"/>
+      <c r="AZ30" s="24"/>
+      <c r="BA30" s="24"/>
     </row>
     <row r="32" spans="2:53" x14ac:dyDescent="0.2">
       <c r="AM32" t="s">
@@ -3846,15 +3898,15 @@
     </row>
     <row r="34" spans="2:46" x14ac:dyDescent="0.2">
       <c r="K34" s="1"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="24"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="24"/>
+      <c r="W34" s="25"/>
+      <c r="X34" s="25"/>
+      <c r="Y34" s="25"/>
       <c r="AM34">
         <v>0.42899999999999999</v>
       </c>
@@ -3882,15 +3934,15 @@
     </row>
     <row r="35" spans="2:46" x14ac:dyDescent="0.2">
       <c r="K35" s="1"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="22"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="22"/>
-      <c r="X35" s="22"/>
-      <c r="Y35" s="22"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="24"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+      <c r="Y35" s="23"/>
       <c r="AM35">
         <v>0.56999999999999995</v>
       </c>
@@ -3930,17 +3982,17 @@
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="Q36" s="29" t="s">
+      <c r="Q36" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="23"/>
-      <c r="X36" s="23"/>
-      <c r="Y36" s="23"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24"/>
       <c r="AM36">
         <v>0.54900000000000004</v>
       </c>
@@ -3997,15 +4049,15 @@
       <c r="O37" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="23"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
+      <c r="V37" s="24"/>
+      <c r="W37" s="24"/>
+      <c r="X37" s="24"/>
+      <c r="Y37" s="24"/>
       <c r="AM37">
         <v>0.55600000000000005</v>
       </c>
@@ -4060,15 +4112,15 @@
       <c r="O38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="23"/>
-      <c r="S38" s="23"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="25"/>
-      <c r="V38" s="23"/>
-      <c r="W38" s="23"/>
-      <c r="X38" s="23"/>
-      <c r="Y38" s="23"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+      <c r="Y38" s="24"/>
       <c r="AM38">
         <v>0.59899999999999998</v>
       </c>
@@ -4114,15 +4166,15 @@
       <c r="O39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="25"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="23"/>
-      <c r="X39" s="23"/>
-      <c r="Y39" s="23"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="24"/>
+      <c r="W39" s="24"/>
+      <c r="X39" s="24"/>
+      <c r="Y39" s="24"/>
       <c r="AM39">
         <v>0.57399999999999995</v>
       </c>
@@ -4178,12 +4230,12 @@
       <c r="S40" s="3">
         <v>0.97642700000000004</v>
       </c>
-      <c r="T40" s="23"/>
-      <c r="U40" s="23"/>
-      <c r="V40" s="23"/>
-      <c r="W40" s="23"/>
-      <c r="X40" s="23"/>
-      <c r="Y40" s="23"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="24"/>
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="24"/>
       <c r="AM40">
         <v>0.55800000000000005</v>
       </c>
@@ -4211,15 +4263,15 @@
     </row>
     <row r="41" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="Q41" s="23"/>
-      <c r="R41" s="23"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="23"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="23"/>
-      <c r="X41" s="23"/>
-      <c r="Y41" s="23"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="24"/>
       <c r="AM41">
         <v>0.625</v>
       </c>
@@ -4246,15 +4298,15 @@
       </c>
     </row>
     <row r="42" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="24"/>
       <c r="AM42">
         <v>0.57299999999999995</v>
       </c>
@@ -4289,24 +4341,24 @@
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
       <c r="K43" s="20" t="s">
         <v>60</v>
       </c>
       <c r="L43" s="20"/>
       <c r="M43" s="20"/>
-      <c r="Q43" s="29" t="s">
+      <c r="Q43" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="23"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="23"/>
-      <c r="X43" s="23"/>
-      <c r="Y43" s="23"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
+      <c r="T43" s="30"/>
+      <c r="U43" s="24"/>
+      <c r="V43" s="24"/>
+      <c r="W43" s="24"/>
+      <c r="X43" s="24"/>
+      <c r="Y43" s="24"/>
       <c r="AM43">
         <v>0.45</v>
       </c>
@@ -4351,17 +4403,17 @@
       <c r="O44" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Q44" s="23" t="s">
+      <c r="Q44" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="25"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="23"/>
-      <c r="Y44" s="23"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="24"/>
+      <c r="W44" s="24"/>
+      <c r="X44" s="24"/>
+      <c r="Y44" s="24"/>
       <c r="AM44">
         <v>0.54</v>
       </c>
@@ -4414,15 +4466,15 @@
         <v>0.50221300000000002</v>
       </c>
       <c r="O45" s="7"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="23"/>
-      <c r="V45" s="23"/>
-      <c r="W45" s="23"/>
-      <c r="X45" s="23"/>
-      <c r="Y45" s="23"/>
+      <c r="Q45" s="24"/>
+      <c r="R45" s="24"/>
+      <c r="S45" s="24"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="24"/>
+      <c r="V45" s="24"/>
+      <c r="W45" s="24"/>
+      <c r="X45" s="24"/>
+      <c r="Y45" s="24"/>
       <c r="AM45">
         <v>0.55900000000000005</v>
       </c>
@@ -4475,15 +4527,15 @@
         <v>0.499114</v>
       </c>
       <c r="O46" s="7"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="23"/>
-      <c r="S46" s="23"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="23"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="23"/>
-      <c r="X46" s="23"/>
-      <c r="Y46" s="23"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="24"/>
       <c r="AM46">
         <v>0.47599999999999998</v>
       </c>
@@ -4548,12 +4600,12 @@
       <c r="S47" s="18">
         <v>0.64534199999999997</v>
       </c>
-      <c r="T47" s="23"/>
-      <c r="U47" s="23"/>
-      <c r="V47" s="23"/>
-      <c r="W47" s="23"/>
-      <c r="X47" s="23"/>
-      <c r="Y47" s="23"/>
+      <c r="T47" s="24"/>
+      <c r="U47" s="24"/>
+      <c r="V47" s="24"/>
+      <c r="W47" s="24"/>
+      <c r="X47" s="24"/>
+      <c r="Y47" s="24"/>
       <c r="AM47">
         <v>0.55300000000000005</v>
       </c>
@@ -4580,15 +4632,15 @@
       </c>
     </row>
     <row r="48" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q48" s="23"/>
-      <c r="R48" s="23"/>
-      <c r="S48" s="23"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="23"/>
-      <c r="V48" s="23"/>
-      <c r="W48" s="23"/>
-      <c r="X48" s="23"/>
-      <c r="Y48" s="23"/>
+      <c r="Q48" s="24"/>
+      <c r="R48" s="24"/>
+      <c r="S48" s="24"/>
+      <c r="T48" s="24"/>
+      <c r="U48" s="24"/>
+      <c r="V48" s="24"/>
+      <c r="W48" s="24"/>
+      <c r="X48" s="24"/>
+      <c r="Y48" s="24"/>
       <c r="AM48">
         <v>0.59099999999999997</v>
       </c>
@@ -4618,15 +4670,15 @@
       <c r="B49" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Q49" s="23"/>
-      <c r="R49" s="23"/>
-      <c r="S49" s="23"/>
-      <c r="T49" s="23"/>
-      <c r="U49" s="23"/>
-      <c r="V49" s="23"/>
-      <c r="W49" s="23"/>
-      <c r="X49" s="23"/>
-      <c r="Y49" s="23"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
+      <c r="S49" s="24"/>
+      <c r="T49" s="24"/>
+      <c r="U49" s="24"/>
+      <c r="V49" s="24"/>
+      <c r="W49" s="24"/>
+      <c r="X49" s="24"/>
+      <c r="Y49" s="24"/>
       <c r="AM49">
         <v>0.59499999999999997</v>
       </c>
@@ -4664,23 +4716,23 @@
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
-      <c r="I50" s="28" t="s">
+      <c r="I50" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
-      <c r="Q50" s="23"/>
-      <c r="R50" s="23"/>
-      <c r="S50" s="23"/>
-      <c r="T50" s="23"/>
-      <c r="U50" s="25"/>
-      <c r="V50" s="23"/>
-      <c r="W50" s="23"/>
-      <c r="X50" s="23"/>
-      <c r="Y50" s="23"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="Q50" s="24"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="24"/>
+      <c r="T50" s="24"/>
+      <c r="U50" s="26"/>
+      <c r="V50" s="24"/>
+      <c r="W50" s="24"/>
+      <c r="X50" s="24"/>
+      <c r="Y50" s="24"/>
       <c r="AM50">
         <v>0.63200000000000001</v>
       </c>
@@ -4722,15 +4774,15 @@
       <c r="G51">
         <v>0.15489900000000001</v>
       </c>
-      <c r="Q51" s="23"/>
-      <c r="R51" s="23"/>
-      <c r="S51" s="23"/>
-      <c r="T51" s="23"/>
-      <c r="U51" s="23"/>
-      <c r="V51" s="23"/>
-      <c r="W51" s="23"/>
-      <c r="X51" s="23"/>
-      <c r="Y51" s="23"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="24"/>
+      <c r="T51" s="24"/>
+      <c r="U51" s="24"/>
+      <c r="V51" s="24"/>
+      <c r="W51" s="24"/>
+      <c r="X51" s="24"/>
+      <c r="Y51" s="24"/>
       <c r="AM51">
         <v>0.58799999999999997</v>
       </c>
@@ -4772,15 +4824,15 @@
       <c r="G52">
         <v>0.31349399999999999</v>
       </c>
-      <c r="Q52" s="23"/>
-      <c r="R52" s="23"/>
-      <c r="S52" s="23"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="23"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="23"/>
-      <c r="X52" s="23"/>
-      <c r="Y52" s="23"/>
+      <c r="Q52" s="24"/>
+      <c r="R52" s="24"/>
+      <c r="S52" s="24"/>
+      <c r="T52" s="24"/>
+      <c r="U52" s="24"/>
+      <c r="V52" s="24"/>
+      <c r="W52" s="24"/>
+      <c r="X52" s="24"/>
+      <c r="Y52" s="24"/>
       <c r="AM52">
         <v>0.55600000000000005</v>
       </c>
@@ -4807,15 +4859,15 @@
       </c>
     </row>
     <row r="53" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q53" s="23"/>
-      <c r="R53" s="23"/>
-      <c r="S53" s="23"/>
-      <c r="T53" s="23"/>
-      <c r="U53" s="23"/>
-      <c r="V53" s="23"/>
-      <c r="W53" s="23"/>
-      <c r="X53" s="23"/>
-      <c r="Y53" s="23"/>
+      <c r="Q53" s="24"/>
+      <c r="R53" s="24"/>
+      <c r="S53" s="24"/>
+      <c r="T53" s="24"/>
+      <c r="U53" s="24"/>
+      <c r="V53" s="24"/>
+      <c r="W53" s="24"/>
+      <c r="X53" s="24"/>
+      <c r="Y53" s="24"/>
       <c r="AM53">
         <v>0.52500000000000002</v>
       </c>
@@ -4842,15 +4894,15 @@
       </c>
     </row>
     <row r="54" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q54" s="23"/>
-      <c r="R54" s="23"/>
-      <c r="S54" s="23"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="23"/>
-      <c r="V54" s="23"/>
-      <c r="W54" s="23"/>
-      <c r="X54" s="23"/>
-      <c r="Y54" s="23"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="24"/>
+      <c r="T54" s="24"/>
+      <c r="U54" s="24"/>
+      <c r="V54" s="24"/>
+      <c r="W54" s="24"/>
+      <c r="X54" s="24"/>
+      <c r="Y54" s="24"/>
       <c r="AM54">
         <v>0.60399999999999998</v>
       </c>
@@ -4877,15 +4929,15 @@
       </c>
     </row>
     <row r="55" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q55" s="23"/>
-      <c r="R55" s="23"/>
-      <c r="S55" s="23"/>
-      <c r="T55" s="23"/>
-      <c r="U55" s="23"/>
-      <c r="V55" s="23"/>
-      <c r="W55" s="23"/>
-      <c r="X55" s="23"/>
-      <c r="Y55" s="23"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="24"/>
+      <c r="T55" s="24"/>
+      <c r="U55" s="24"/>
+      <c r="V55" s="24"/>
+      <c r="W55" s="24"/>
+      <c r="X55" s="24"/>
+      <c r="Y55" s="24"/>
       <c r="AM55">
         <v>0.6</v>
       </c>
@@ -4912,81 +4964,81 @@
       </c>
     </row>
     <row r="56" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q56" s="23"/>
-      <c r="R56" s="23"/>
-      <c r="S56" s="23"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="23"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="23"/>
-      <c r="X56" s="23"/>
-      <c r="Y56" s="23"/>
+      <c r="Q56" s="24"/>
+      <c r="R56" s="24"/>
+      <c r="S56" s="24"/>
+      <c r="T56" s="24"/>
+      <c r="U56" s="24"/>
+      <c r="V56" s="24"/>
+      <c r="W56" s="24"/>
+      <c r="X56" s="24"/>
+      <c r="Y56" s="24"/>
     </row>
     <row r="57" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q57" s="23"/>
-      <c r="R57" s="23"/>
-      <c r="S57" s="23"/>
-      <c r="T57" s="23"/>
-      <c r="U57" s="23"/>
-      <c r="V57" s="23"/>
-      <c r="W57" s="23"/>
-      <c r="X57" s="23"/>
-      <c r="Y57" s="23"/>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="24"/>
+      <c r="S57" s="24"/>
+      <c r="T57" s="24"/>
+      <c r="U57" s="24"/>
+      <c r="V57" s="24"/>
+      <c r="W57" s="24"/>
+      <c r="X57" s="24"/>
+      <c r="Y57" s="24"/>
     </row>
     <row r="58" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q58" s="23"/>
-      <c r="R58" s="23"/>
-      <c r="S58" s="23"/>
-      <c r="T58" s="23"/>
-      <c r="U58" s="23"/>
-      <c r="V58" s="23"/>
-      <c r="W58" s="23"/>
-      <c r="X58" s="23"/>
-      <c r="Y58" s="23"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="24"/>
+      <c r="S58" s="24"/>
+      <c r="T58" s="24"/>
+      <c r="U58" s="24"/>
+      <c r="V58" s="24"/>
+      <c r="W58" s="24"/>
+      <c r="X58" s="24"/>
+      <c r="Y58" s="24"/>
     </row>
     <row r="59" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q59" s="23"/>
-      <c r="R59" s="23"/>
-      <c r="S59" s="23"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="23"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="23"/>
-      <c r="X59" s="23"/>
-      <c r="Y59" s="23"/>
+      <c r="Q59" s="24"/>
+      <c r="R59" s="24"/>
+      <c r="S59" s="24"/>
+      <c r="T59" s="24"/>
+      <c r="U59" s="24"/>
+      <c r="V59" s="24"/>
+      <c r="W59" s="24"/>
+      <c r="X59" s="24"/>
+      <c r="Y59" s="24"/>
     </row>
     <row r="60" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q60" s="23"/>
-      <c r="R60" s="23"/>
-      <c r="S60" s="23"/>
-      <c r="T60" s="23"/>
-      <c r="U60" s="23"/>
-      <c r="V60" s="23"/>
-      <c r="W60" s="23"/>
-      <c r="X60" s="23"/>
-      <c r="Y60" s="23"/>
+      <c r="Q60" s="24"/>
+      <c r="R60" s="24"/>
+      <c r="S60" s="24"/>
+      <c r="T60" s="24"/>
+      <c r="U60" s="24"/>
+      <c r="V60" s="24"/>
+      <c r="W60" s="24"/>
+      <c r="X60" s="24"/>
+      <c r="Y60" s="24"/>
     </row>
     <row r="61" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q61" s="23"/>
-      <c r="R61" s="23"/>
-      <c r="S61" s="23"/>
-      <c r="T61" s="23"/>
-      <c r="U61" s="23"/>
-      <c r="V61" s="23"/>
-      <c r="W61" s="23"/>
-      <c r="X61" s="23"/>
-      <c r="Y61" s="23"/>
+      <c r="Q61" s="24"/>
+      <c r="R61" s="24"/>
+      <c r="S61" s="24"/>
+      <c r="T61" s="24"/>
+      <c r="U61" s="24"/>
+      <c r="V61" s="24"/>
+      <c r="W61" s="24"/>
+      <c r="X61" s="24"/>
+      <c r="Y61" s="24"/>
     </row>
     <row r="62" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="Q62" s="23"/>
-      <c r="R62" s="23"/>
-      <c r="S62" s="23"/>
-      <c r="T62" s="23"/>
-      <c r="U62" s="23"/>
-      <c r="V62" s="23"/>
-      <c r="W62" s="23"/>
-      <c r="X62" s="23"/>
-      <c r="Y62" s="23"/>
+      <c r="Q62" s="24"/>
+      <c r="R62" s="24"/>
+      <c r="S62" s="24"/>
+      <c r="T62" s="24"/>
+      <c r="U62" s="24"/>
+      <c r="V62" s="24"/>
+      <c r="W62" s="24"/>
+      <c r="X62" s="24"/>
+      <c r="Y62" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5010,45 +5062,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F016DC3-7647-EC40-938C-4348D53868B2}">
-  <dimension ref="A1:AC43"/>
+  <dimension ref="A1:AH53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="93" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="X24" zoomScale="109" workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="L1" s="30" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="L1" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="V1" s="30" t="s">
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="V1" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
@@ -5086,82 +5138,82 @@
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="34" t="s">
         <v>184</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="O3" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="Q3" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="R3" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S3" s="34" t="s">
         <v>184</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="V3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="33" t="s">
+      <c r="W3" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="X3" s="33" t="s">
+      <c r="X3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="Y3" s="33" t="s">
+      <c r="Y3" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="Z3" s="33" t="s">
+      <c r="Z3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="33" t="s">
+      <c r="AA3" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="AB3" s="33" t="s">
+      <c r="AB3" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="34" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5169,39 +5221,39 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
       <c r="K4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="34">
         <v>0.47099999999999997</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="34">
         <v>0.34100000000000003</v>
       </c>
-      <c r="O4" s="33" t="s">
+      <c r="O4" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="33">
+      <c r="P4" s="34">
         <v>0.27100000000000002</v>
       </c>
-      <c r="Q4" s="33" t="s">
+      <c r="Q4" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="R4" s="33">
+      <c r="R4" s="34">
         <v>0.34100000000000003</v>
       </c>
-      <c r="S4" s="33" t="s">
+      <c r="S4" s="34" t="s">
         <v>95</v>
       </c>
       <c r="U4" s="7" t="s">
@@ -5236,39 +5288,39 @@
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
       <c r="K5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="33">
+      <c r="L5" s="34">
         <v>0.42899999999999999</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="34">
         <v>0.27200000000000002</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="O5" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="33">
+      <c r="P5" s="34">
         <v>0.192</v>
       </c>
-      <c r="Q5" s="33" t="s">
+      <c r="Q5" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="R5" s="33">
+      <c r="R5" s="34">
         <v>0.27200000000000002</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="S5" s="34" t="s">
         <v>99</v>
       </c>
       <c r="U5" s="7" t="s">
@@ -5303,39 +5355,39 @@
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="K6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="33">
+      <c r="L6" s="34">
         <v>0.56999999999999995</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="34">
         <v>0.442</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="O6" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="P6" s="33">
+      <c r="P6" s="34">
         <v>0.41099999999999998</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="Q6" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="R6" s="33">
+      <c r="R6" s="34">
         <v>0.442</v>
       </c>
-      <c r="S6" s="33" t="s">
+      <c r="S6" s="34" t="s">
         <v>103</v>
       </c>
       <c r="U6" s="7" t="s">
@@ -5370,39 +5422,39 @@
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="34">
         <v>0.54900000000000004</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="34">
         <v>0.44800000000000001</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="O7" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="P7" s="33">
+      <c r="P7" s="34">
         <v>0.41899999999999998</v>
       </c>
-      <c r="Q7" s="33" t="s">
+      <c r="Q7" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="R7" s="33">
+      <c r="R7" s="34">
         <v>0.44800000000000001</v>
       </c>
-      <c r="S7" s="33" t="s">
+      <c r="S7" s="34" t="s">
         <v>107</v>
       </c>
       <c r="U7" s="7" t="s">
@@ -5437,39 +5489,39 @@
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="K8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="34">
         <v>0.55600000000000005</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="34">
         <v>0.41599999999999998</v>
       </c>
-      <c r="O8" s="33" t="s">
+      <c r="O8" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="33">
+      <c r="P8" s="34">
         <v>0.38500000000000001</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="R8" s="33">
+      <c r="R8" s="34">
         <v>0.41599999999999998</v>
       </c>
-      <c r="S8" s="33" t="s">
+      <c r="S8" s="34" t="s">
         <v>111</v>
       </c>
       <c r="U8" s="7" t="s">
@@ -5504,39 +5556,39 @@
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
       <c r="K9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="34">
         <v>0.59899999999999998</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="34">
         <v>0.45900000000000002</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="O9" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="P9" s="33">
+      <c r="P9" s="34">
         <v>0.442</v>
       </c>
-      <c r="Q9" s="33" t="s">
+      <c r="Q9" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="R9" s="33">
+      <c r="R9" s="34">
         <v>0.45900000000000002</v>
       </c>
-      <c r="S9" s="33" t="s">
+      <c r="S9" s="34" t="s">
         <v>115</v>
       </c>
       <c r="U9" s="7" t="s">
@@ -5571,39 +5623,39 @@
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
       <c r="K10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="34">
         <v>0.57399999999999995</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="34">
         <v>0.433</v>
       </c>
-      <c r="O10" s="33" t="s">
+      <c r="O10" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="P10" s="33">
+      <c r="P10" s="34">
         <v>0.40899999999999997</v>
       </c>
-      <c r="Q10" s="33" t="s">
+      <c r="Q10" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="R10" s="33">
+      <c r="R10" s="34">
         <v>0.433</v>
       </c>
-      <c r="S10" s="33" t="s">
+      <c r="S10" s="34" t="s">
         <v>119</v>
       </c>
       <c r="U10" s="7" t="s">
@@ -5638,39 +5690,39 @@
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
       <c r="K11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="34">
         <v>0.55800000000000005</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="34">
         <v>0.43099999999999999</v>
       </c>
-      <c r="O11" s="33" t="s">
+      <c r="O11" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="P11" s="33">
+      <c r="P11" s="34">
         <v>0.41199999999999998</v>
       </c>
-      <c r="Q11" s="33" t="s">
+      <c r="Q11" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="R11" s="33">
+      <c r="R11" s="34">
         <v>0.43099999999999999</v>
       </c>
-      <c r="S11" s="33" t="s">
+      <c r="S11" s="34" t="s">
         <v>123</v>
       </c>
       <c r="U11" s="7" t="s">
@@ -5705,39 +5757,39 @@
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="K12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="34">
         <v>0.625</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="M12" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="34">
         <v>0.50700000000000001</v>
       </c>
-      <c r="O12" s="33" t="s">
+      <c r="O12" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="P12" s="33">
+      <c r="P12" s="34">
         <v>0.48799999999999999</v>
       </c>
-      <c r="Q12" s="33" t="s">
+      <c r="Q12" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="R12" s="33">
+      <c r="R12" s="34">
         <v>0.50700000000000001</v>
       </c>
-      <c r="S12" s="33" t="s">
+      <c r="S12" s="34" t="s">
         <v>125</v>
       </c>
       <c r="U12" s="7" t="s">
@@ -5772,39 +5824,39 @@
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
       <c r="K13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="34">
         <v>0.57299999999999995</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="34">
         <v>0.52600000000000002</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O13" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="P13" s="33">
+      <c r="P13" s="34">
         <v>0.51800000000000002</v>
       </c>
-      <c r="Q13" s="33" t="s">
+      <c r="Q13" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="R13" s="33">
+      <c r="R13" s="34">
         <v>0.52600000000000002</v>
       </c>
-      <c r="S13" s="33" t="s">
+      <c r="S13" s="34" t="s">
         <v>130</v>
       </c>
       <c r="U13" s="7" t="s">
@@ -5839,39 +5891,39 @@
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="K14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="34">
         <v>0.45</v>
       </c>
-      <c r="M14" s="33" t="s">
+      <c r="M14" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="34">
         <v>0.29799999999999999</v>
       </c>
-      <c r="O14" s="33" t="s">
+      <c r="O14" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="P14" s="33">
+      <c r="P14" s="34">
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q14" s="33" t="s">
+      <c r="Q14" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="R14" s="33">
+      <c r="R14" s="34">
         <v>0.29799999999999999</v>
       </c>
-      <c r="S14" s="33" t="s">
+      <c r="S14" s="34" t="s">
         <v>134</v>
       </c>
       <c r="U14" s="7" t="s">
@@ -5906,39 +5958,39 @@
       <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
       <c r="K15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="34">
         <v>0.54</v>
       </c>
-      <c r="M15" s="33" t="s">
+      <c r="M15" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="34">
         <v>0.39900000000000002</v>
       </c>
-      <c r="O15" s="33" t="s">
+      <c r="O15" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="P15" s="33">
+      <c r="P15" s="34">
         <v>0.36499999999999999</v>
       </c>
-      <c r="Q15" s="33" t="s">
+      <c r="Q15" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="R15" s="33">
+      <c r="R15" s="34">
         <v>0.39900000000000002</v>
       </c>
-      <c r="S15" s="33" t="s">
+      <c r="S15" s="34" t="s">
         <v>138</v>
       </c>
       <c r="U15" s="7" t="s">
@@ -5973,39 +6025,39 @@
       <c r="A16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="K16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="33">
+      <c r="L16" s="34">
         <v>0.55900000000000005</v>
       </c>
-      <c r="M16" s="33" t="s">
+      <c r="M16" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="34">
         <v>0.42299999999999999</v>
       </c>
-      <c r="O16" s="33" t="s">
+      <c r="O16" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="P16" s="33">
+      <c r="P16" s="34">
         <v>0.39500000000000002</v>
       </c>
-      <c r="Q16" s="33" t="s">
+      <c r="Q16" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="R16" s="33">
+      <c r="R16" s="34">
         <v>0.42299999999999999</v>
       </c>
-      <c r="S16" s="33" t="s">
+      <c r="S16" s="34" t="s">
         <v>142</v>
       </c>
       <c r="U16" s="7" t="s">
@@ -6036,43 +6088,43 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="K17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="33">
+      <c r="L17" s="34">
         <v>0.47599999999999998</v>
       </c>
-      <c r="M17" s="33" t="s">
+      <c r="M17" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="34">
         <v>0.34799999999999998</v>
       </c>
-      <c r="O17" s="33" t="s">
+      <c r="O17" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="P17" s="33">
+      <c r="P17" s="34">
         <v>0.28100000000000003</v>
       </c>
-      <c r="Q17" s="33" t="s">
+      <c r="Q17" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="R17" s="33">
+      <c r="R17" s="34">
         <v>0.34799999999999998</v>
       </c>
-      <c r="S17" s="33" t="s">
+      <c r="S17" s="34" t="s">
         <v>146</v>
       </c>
       <c r="U17" s="7" t="s">
@@ -6103,43 +6155,43 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="34">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M18" s="33" t="s">
+      <c r="M18" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="34">
         <v>0.44900000000000001</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="O18" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="P18" s="33">
+      <c r="P18" s="34">
         <v>0.42199999999999999</v>
       </c>
-      <c r="Q18" s="33" t="s">
+      <c r="Q18" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="R18" s="33">
+      <c r="R18" s="34">
         <v>0.44900000000000001</v>
       </c>
-      <c r="S18" s="33" t="s">
+      <c r="S18" s="34" t="s">
         <v>150</v>
       </c>
       <c r="U18" s="7" t="s">
@@ -6170,43 +6222,43 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
       <c r="K19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="34">
         <v>0.59099999999999997</v>
       </c>
-      <c r="M19" s="33" t="s">
+      <c r="M19" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="N19" s="33">
+      <c r="N19" s="34">
         <v>0.46400000000000002</v>
       </c>
-      <c r="O19" s="33" t="s">
+      <c r="O19" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="P19" s="33">
+      <c r="P19" s="34">
         <v>0.44600000000000001</v>
       </c>
-      <c r="Q19" s="33" t="s">
+      <c r="Q19" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="R19" s="33">
+      <c r="R19" s="34">
         <v>0.46400000000000002</v>
       </c>
-      <c r="S19" s="33" t="s">
+      <c r="S19" s="34" t="s">
         <v>154</v>
       </c>
       <c r="U19" s="7" t="s">
@@ -6237,43 +6289,43 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
       <c r="K20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="34">
         <v>0.59499999999999997</v>
       </c>
-      <c r="M20" s="33" t="s">
+      <c r="M20" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="34">
         <v>0.46100000000000002</v>
       </c>
-      <c r="O20" s="33" t="s">
+      <c r="O20" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="34">
         <v>0.442</v>
       </c>
-      <c r="Q20" s="33" t="s">
+      <c r="Q20" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="R20" s="33">
+      <c r="R20" s="34">
         <v>0.46100000000000002</v>
       </c>
-      <c r="S20" s="33" t="s">
+      <c r="S20" s="34" t="s">
         <v>158</v>
       </c>
       <c r="U20" s="7" t="s">
@@ -6304,43 +6356,43 @@
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
       <c r="K21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="33">
+      <c r="L21" s="34">
         <v>0.63200000000000001</v>
       </c>
-      <c r="M21" s="33" t="s">
+      <c r="M21" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="N21" s="33">
+      <c r="N21" s="34">
         <v>0.50900000000000001</v>
       </c>
-      <c r="O21" s="33" t="s">
+      <c r="O21" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="P21" s="33">
+      <c r="P21" s="34">
         <v>0.48699999999999999</v>
       </c>
-      <c r="Q21" s="33" t="s">
+      <c r="Q21" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="R21" s="33">
+      <c r="R21" s="34">
         <v>0.50900000000000001</v>
       </c>
-      <c r="S21" s="33" t="s">
+      <c r="S21" s="34" t="s">
         <v>162</v>
       </c>
       <c r="U21" s="7" t="s">
@@ -6371,43 +6423,43 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
       <c r="K22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="33">
+      <c r="L22" s="34">
         <v>0.58799999999999997</v>
       </c>
-      <c r="M22" s="33" t="s">
+      <c r="M22" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="N22" s="33">
+      <c r="N22" s="34">
         <v>0.51900000000000002</v>
       </c>
-      <c r="O22" s="33" t="s">
+      <c r="O22" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="P22" s="33">
+      <c r="P22" s="34">
         <v>0.50900000000000001</v>
       </c>
-      <c r="Q22" s="33" t="s">
+      <c r="Q22" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="R22" s="33">
+      <c r="R22" s="34">
         <v>0.51900000000000002</v>
       </c>
-      <c r="S22" s="33" t="s">
+      <c r="S22" s="34" t="s">
         <v>166</v>
       </c>
       <c r="U22" s="7" t="s">
@@ -6438,43 +6490,43 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
       <c r="K23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="33">
+      <c r="L23" s="34">
         <v>0.55600000000000005</v>
       </c>
-      <c r="M23" s="33" t="s">
+      <c r="M23" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="N23" s="33">
+      <c r="N23" s="34">
         <v>0.41799999999999998</v>
       </c>
-      <c r="O23" s="33" t="s">
+      <c r="O23" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="P23" s="33">
+      <c r="P23" s="34">
         <v>0.39200000000000002</v>
       </c>
-      <c r="Q23" s="33" t="s">
+      <c r="Q23" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="R23" s="33">
+      <c r="R23" s="34">
         <v>0.41799999999999998</v>
       </c>
-      <c r="S23" s="33" t="s">
+      <c r="S23" s="34" t="s">
         <v>169</v>
       </c>
       <c r="U23" s="7" t="s">
@@ -6505,43 +6557,43 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
       <c r="K24" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="33">
+      <c r="L24" s="34">
         <v>0.52500000000000002</v>
       </c>
-      <c r="M24" s="33" t="s">
+      <c r="M24" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="N24" s="33">
+      <c r="N24" s="34">
         <v>0.39500000000000002</v>
       </c>
-      <c r="O24" s="33" t="s">
+      <c r="O24" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="P24" s="33">
+      <c r="P24" s="34">
         <v>0.36</v>
       </c>
-      <c r="Q24" s="33" t="s">
+      <c r="Q24" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="R24" s="33">
+      <c r="R24" s="34">
         <v>0.39500000000000002</v>
       </c>
-      <c r="S24" s="33" t="s">
+      <c r="S24" s="34" t="s">
         <v>173</v>
       </c>
       <c r="U24" s="7" t="s">
@@ -6572,43 +6624,43 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
       <c r="K25" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="L25" s="33">
+      <c r="L25" s="34">
         <v>0.60399999999999998</v>
       </c>
-      <c r="M25" s="33" t="s">
+      <c r="M25" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="N25" s="33">
+      <c r="N25" s="34">
         <v>0.45900000000000002</v>
       </c>
-      <c r="O25" s="33" t="s">
+      <c r="O25" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="P25" s="33">
+      <c r="P25" s="34">
         <v>0.42199999999999999</v>
       </c>
-      <c r="Q25" s="33" t="s">
+      <c r="Q25" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="R25" s="33">
+      <c r="R25" s="34">
         <v>0.45900000000000002</v>
       </c>
-      <c r="S25" s="33" t="s">
+      <c r="S25" s="34" t="s">
         <v>176</v>
       </c>
       <c r="U25" s="7" t="s">
@@ -6639,43 +6691,43 @@
         <v>266</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
       <c r="K26" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="L26" s="33">
+      <c r="L26" s="34">
         <v>0.6</v>
       </c>
-      <c r="M26" s="33" t="s">
+      <c r="M26" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="N26" s="33">
+      <c r="N26" s="34">
         <v>0.45300000000000001</v>
       </c>
-      <c r="O26" s="33" t="s">
+      <c r="O26" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="P26" s="33">
+      <c r="P26" s="34">
         <v>0.437</v>
       </c>
-      <c r="Q26" s="33" t="s">
+      <c r="Q26" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="R26" s="33">
+      <c r="R26" s="34">
         <v>0.45300000000000001</v>
       </c>
-      <c r="S26" s="33" t="s">
+      <c r="S26" s="34" t="s">
         <v>178</v>
       </c>
       <c r="U26" s="17" t="s">
@@ -6706,7 +6758,29 @@
         <v>270</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="Z28" s="37"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AA30" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB30" s="31"/>
+      <c r="AC30" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="AD30" s="31"/>
+      <c r="AF30" t="s">
+        <v>322</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>323</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>84</v>
       </c>
@@ -6716,61 +6790,135 @@
       <c r="P31" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="W31" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="X31" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y31" s="38"/>
+      <c r="Z31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA31">
+        <v>0.23</v>
+      </c>
+      <c r="AB31">
+        <v>0.314</v>
+      </c>
+      <c r="AC31">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AD31">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="AE31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF31">
+        <f>AA31-AC31</f>
+        <v>6.2E-2</v>
+      </c>
+      <c r="AG31">
+        <f>AB31-AD31</f>
+        <v>5.6999999999999995E-2</v>
+      </c>
+      <c r="AH31">
+        <f>AF31+AG31</f>
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="F32" s="34" t="s">
+      <c r="F32" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="34" t="s">
+      <c r="G32" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="L32" s="34" t="s">
+      <c r="L32" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="M32" s="34" t="s">
+      <c r="M32" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="N32" s="34" t="s">
+      <c r="N32" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="O32" s="34" t="s">
+      <c r="O32" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="P32" s="34" t="s">
+      <c r="P32" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="Q32" s="34" t="s">
+      <c r="Q32" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="R32" s="34" t="s">
+      <c r="R32" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="S32" s="34" t="s">
+      <c r="S32" s="35" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W32" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="X32" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y32" s="38"/>
+      <c r="Z32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA32">
+        <v>0.158</v>
+      </c>
+      <c r="AB32">
+        <v>0.23</v>
+      </c>
+      <c r="AC32">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AD32">
+        <v>0.215</v>
+      </c>
+      <c r="AE32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF32">
+        <f>AA32-AC32</f>
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="AG32">
+        <f>AB32-AD32</f>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="AH32">
+        <f>AF32+AG32</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
@@ -6822,8 +6970,45 @@
       <c r="S33" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W33" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="X33" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y33" s="38"/>
+      <c r="Z33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA33">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="AB33">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="AC33">
+        <v>0.308</v>
+      </c>
+      <c r="AD33">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="AE33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" ref="AF33:AF41" si="0">AA33-AC33</f>
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AG33">
+        <f>AB33-AD33</f>
+        <v>4.7000000000000042E-2</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" ref="AH33:AH41" si="1">AF33+AG33</f>
+        <v>0.10600000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
@@ -6875,8 +7060,45 @@
       <c r="S34" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W34" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="X34" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y34" s="38"/>
+      <c r="Z34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA34">
+        <v>0.374</v>
+      </c>
+      <c r="AB34">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="AC34">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="AD34">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="AE34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999992E-2</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" ref="AG34:AG41" si="2">AB34-AD34</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="1"/>
+        <v>9.3000000000000027E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>7</v>
       </c>
@@ -6928,13 +7150,87 @@
       <c r="S35" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W35" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="X35" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y35" s="38"/>
+      <c r="Z35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA35">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="AB35">
+        <v>0.43</v>
+      </c>
+      <c r="AC35">
+        <v>0.308</v>
+      </c>
+      <c r="AD35">
+        <v>0.41</v>
+      </c>
+      <c r="AE35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF35">
+        <f>AA35-AC35</f>
+        <v>3.3000000000000029E-2</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="2"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="1"/>
+        <v>5.3000000000000047E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L36" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W36" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="X36" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y36" s="38"/>
+      <c r="Z36" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA36">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="AB36">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="AC36">
+        <v>0.33</v>
+      </c>
+      <c r="AD36">
+        <v>0.433</v>
+      </c>
+      <c r="AE36" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="0"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="2"/>
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" si="1"/>
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L37">
         <v>0.74099999999999999</v>
       </c>
@@ -6959,42 +7255,153 @@
       <c r="S37" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W37" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="X37" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y37" s="38"/>
+      <c r="Z37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA37">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="AB37">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="AC37">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="AD37">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="AE37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="0"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="2"/>
+        <v>5.4999999999999993E-2</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W38" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="X38" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y38" s="38"/>
+      <c r="Z38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA38">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="AB38">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="AC38">
+        <v>0.307</v>
+      </c>
+      <c r="AD38">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="AE38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="0"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="2"/>
+        <v>4.8000000000000043E-2</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="1"/>
+        <v>0.10900000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="34" t="s">
+      <c r="G39" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="H39" s="34" t="s">
+      <c r="H39" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="I39" s="35" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W39" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="X39" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y39" s="38"/>
+      <c r="Z39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA39">
+        <v>0.443</v>
+      </c>
+      <c r="AB39">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="AC39">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="AD39">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="AE39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="0"/>
+        <v>8.4000000000000019E-2</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="2"/>
+        <v>7.1000000000000008E-2</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="1"/>
+        <v>0.15500000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
@@ -7022,8 +7429,45 @@
       <c r="I40" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W40" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="X40" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y40" s="38"/>
+      <c r="Z40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA40">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="AB40">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="AC40">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="AD40">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="AE40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999988E-2</v>
+      </c>
+      <c r="AG40">
+        <f t="shared" si="2"/>
+        <v>3.400000000000003E-2</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" si="1"/>
+        <v>8.3000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>6</v>
       </c>
@@ -7051,8 +7495,45 @@
       <c r="I41" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="W41" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="X41" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y41" s="38"/>
+      <c r="Z41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA41">
+        <v>0.187</v>
+      </c>
+      <c r="AB41">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AC41">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AD41">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AE41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000006E-2</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="2"/>
+        <v>2.9000000000000026E-2</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="1"/>
+        <v>6.7000000000000032E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>7</v>
       </c>
@@ -7080,9 +7561,16 @@
       <c r="I42" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
+      <c r="W42" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="X42" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z42" s="22"/>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A43" s="36" t="s">
         <v>311</v>
       </c>
       <c r="B43">
@@ -7109,9 +7597,98 @@
       <c r="I43" t="s">
         <v>309</v>
       </c>
+      <c r="W43" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="X43" t="s">
+        <v>234</v>
+      </c>
+      <c r="Z43" s="22"/>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W44" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="X44" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W45" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="X45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W46" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="X46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W47" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="X47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="W48" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="X48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W49" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="X49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W50" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="X50" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W51" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="X51" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W52" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="X52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W53" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="X53" t="s">
+        <v>269</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="AC30:AD30"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="L1:S1"/>

</xml_diff>